<commit_message>
Fill termo de autorização.
</commit_message>
<xml_diff>
--- a/documents/Termo de Autorização - Dissertação-Teses_04_2017.xlsx
+++ b/documents/Termo de Autorização - Dissertação-Teses_04_2017.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lvechi\Desktop\TRABALHO\MODELOS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Doutorado\thesis_project\thesis\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <workbookProtection workbookPassword="CEEB" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="6110"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="6105"/>
   </bookViews>
   <sheets>
     <sheet name="Termo de autorização" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="52">
   <si>
     <t>TERMO DE AUTORIZAÇÃO – DISSERTAÇÃO/TESE</t>
   </si>
@@ -205,11 +205,53 @@
   <si>
     <t>em (data)</t>
   </si>
+  <si>
+    <t>Fernando Henrique de Sá</t>
+  </si>
+  <si>
+    <t>Brasileiro</t>
+  </si>
+  <si>
+    <t>Solteiro</t>
+  </si>
+  <si>
+    <t>Físico de Aceleradores</t>
+  </si>
+  <si>
+    <t>Rua José Pugliesi Filho, 451, ap. 02</t>
+  </si>
+  <si>
+    <t>Campinas</t>
+  </si>
+  <si>
+    <t>SP</t>
+  </si>
+  <si>
+    <t>40532892-8</t>
+  </si>
+  <si>
+    <t>Study of Impedances and Collective Instabilities Applied to Sirius</t>
+  </si>
+  <si>
+    <t>Doutorado</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>abril</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -403,13 +445,94 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -419,87 +542,6 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -869,149 +911,153 @@
   <dimension ref="C1:CG47"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:AJ3"/>
+      <selection activeCell="J28" sqref="J28:K28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="5" width="1.6328125" customWidth="1"/>
-    <col min="6" max="6" width="2.08984375" customWidth="1"/>
-    <col min="7" max="7" width="1.6328125" customWidth="1"/>
-    <col min="8" max="8" width="2.36328125" customWidth="1"/>
-    <col min="9" max="10" width="1.6328125" customWidth="1"/>
-    <col min="11" max="11" width="1.08984375" customWidth="1"/>
-    <col min="12" max="57" width="1.6328125" customWidth="1"/>
-    <col min="58" max="58" width="1.90625" customWidth="1"/>
-    <col min="59" max="95" width="3.90625" customWidth="1"/>
+    <col min="3" max="5" width="1.5703125" customWidth="1"/>
+    <col min="6" max="6" width="2.140625" customWidth="1"/>
+    <col min="7" max="7" width="1.5703125" customWidth="1"/>
+    <col min="8" max="8" width="2.42578125" customWidth="1"/>
+    <col min="9" max="10" width="1.5703125" customWidth="1"/>
+    <col min="11" max="11" width="1.140625" customWidth="1"/>
+    <col min="12" max="57" width="1.5703125" customWidth="1"/>
+    <col min="58" max="58" width="1.85546875" customWidth="1"/>
+    <col min="59" max="95" width="3.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:85" ht="39" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C1" s="47" t="s">
+    <row r="1" spans="3:85" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
-      <c r="L1" s="48"/>
-      <c r="M1" s="48"/>
-      <c r="N1" s="48"/>
-      <c r="O1" s="48"/>
-      <c r="P1" s="48"/>
-      <c r="Q1" s="48"/>
-      <c r="R1" s="48"/>
-      <c r="S1" s="48"/>
-      <c r="T1" s="48"/>
-      <c r="U1" s="48"/>
-      <c r="V1" s="48"/>
-      <c r="W1" s="48"/>
-      <c r="X1" s="48"/>
-      <c r="Y1" s="48"/>
-      <c r="Z1" s="48"/>
-      <c r="AA1" s="48"/>
-      <c r="AB1" s="48"/>
-      <c r="AC1" s="48"/>
-      <c r="AD1" s="48"/>
-      <c r="AE1" s="48"/>
-      <c r="AF1" s="48"/>
-      <c r="AG1" s="48"/>
-      <c r="AH1" s="48"/>
-      <c r="AI1" s="48"/>
-      <c r="AJ1" s="48"/>
-      <c r="AK1" s="48"/>
-      <c r="AL1" s="48"/>
-      <c r="AM1" s="48"/>
-      <c r="AN1" s="48"/>
-      <c r="AO1" s="48"/>
-      <c r="AP1" s="48"/>
-      <c r="AQ1" s="48"/>
-      <c r="AR1" s="48"/>
-      <c r="AS1" s="48"/>
-      <c r="AT1" s="48"/>
-      <c r="AU1" s="48"/>
-      <c r="AV1" s="48"/>
-      <c r="AW1" s="48"/>
-      <c r="AX1" s="48"/>
-      <c r="AY1" s="48"/>
-      <c r="AZ1" s="48"/>
-      <c r="BA1" s="48"/>
-      <c r="BB1" s="48"/>
-      <c r="BC1" s="48"/>
-      <c r="BD1" s="48"/>
-      <c r="BE1" s="48"/>
-      <c r="BF1" s="48"/>
-    </row>
-    <row r="3" spans="3:85" x14ac:dyDescent="0.35">
-      <c r="C3" s="53" t="s">
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
+      <c r="K1" s="51"/>
+      <c r="L1" s="51"/>
+      <c r="M1" s="51"/>
+      <c r="N1" s="51"/>
+      <c r="O1" s="51"/>
+      <c r="P1" s="51"/>
+      <c r="Q1" s="51"/>
+      <c r="R1" s="51"/>
+      <c r="S1" s="51"/>
+      <c r="T1" s="51"/>
+      <c r="U1" s="51"/>
+      <c r="V1" s="51"/>
+      <c r="W1" s="51"/>
+      <c r="X1" s="51"/>
+      <c r="Y1" s="51"/>
+      <c r="Z1" s="51"/>
+      <c r="AA1" s="51"/>
+      <c r="AB1" s="51"/>
+      <c r="AC1" s="51"/>
+      <c r="AD1" s="51"/>
+      <c r="AE1" s="51"/>
+      <c r="AF1" s="51"/>
+      <c r="AG1" s="51"/>
+      <c r="AH1" s="51"/>
+      <c r="AI1" s="51"/>
+      <c r="AJ1" s="51"/>
+      <c r="AK1" s="51"/>
+      <c r="AL1" s="51"/>
+      <c r="AM1" s="51"/>
+      <c r="AN1" s="51"/>
+      <c r="AO1" s="51"/>
+      <c r="AP1" s="51"/>
+      <c r="AQ1" s="51"/>
+      <c r="AR1" s="51"/>
+      <c r="AS1" s="51"/>
+      <c r="AT1" s="51"/>
+      <c r="AU1" s="51"/>
+      <c r="AV1" s="51"/>
+      <c r="AW1" s="51"/>
+      <c r="AX1" s="51"/>
+      <c r="AY1" s="51"/>
+      <c r="AZ1" s="51"/>
+      <c r="BA1" s="51"/>
+      <c r="BB1" s="51"/>
+      <c r="BC1" s="51"/>
+      <c r="BD1" s="51"/>
+      <c r="BE1" s="51"/>
+      <c r="BF1" s="51"/>
+    </row>
+    <row r="3" spans="3:85" x14ac:dyDescent="0.25">
+      <c r="C3" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="53"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
-      <c r="K3" s="37"/>
-      <c r="L3" s="37"/>
-      <c r="M3" s="37"/>
-      <c r="N3" s="37"/>
-      <c r="O3" s="37"/>
-      <c r="P3" s="37"/>
-      <c r="Q3" s="37"/>
-      <c r="R3" s="37"/>
-      <c r="S3" s="37"/>
-      <c r="T3" s="37"/>
-      <c r="U3" s="37"/>
-      <c r="V3" s="37"/>
-      <c r="W3" s="37"/>
-      <c r="X3" s="37"/>
-      <c r="Y3" s="37"/>
-      <c r="Z3" s="37"/>
-      <c r="AA3" s="37"/>
-      <c r="AB3" s="37"/>
-      <c r="AC3" s="37"/>
-      <c r="AD3" s="37"/>
-      <c r="AE3" s="37"/>
-      <c r="AF3" s="37"/>
-      <c r="AG3" s="37"/>
-      <c r="AH3" s="37"/>
-      <c r="AI3" s="37"/>
-      <c r="AJ3" s="37"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="46" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="46"/>
+      <c r="L3" s="46"/>
+      <c r="M3" s="46"/>
+      <c r="N3" s="46"/>
+      <c r="O3" s="46"/>
+      <c r="P3" s="46"/>
+      <c r="Q3" s="46"/>
+      <c r="R3" s="46"/>
+      <c r="S3" s="46"/>
+      <c r="T3" s="46"/>
+      <c r="U3" s="46"/>
+      <c r="V3" s="46"/>
+      <c r="W3" s="46"/>
+      <c r="X3" s="46"/>
+      <c r="Y3" s="46"/>
+      <c r="Z3" s="46"/>
+      <c r="AA3" s="46"/>
+      <c r="AB3" s="46"/>
+      <c r="AC3" s="46"/>
+      <c r="AD3" s="46"/>
+      <c r="AE3" s="46"/>
+      <c r="AF3" s="46"/>
+      <c r="AG3" s="46"/>
+      <c r="AH3" s="46"/>
+      <c r="AI3" s="46"/>
+      <c r="AJ3" s="46"/>
       <c r="AK3" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="AL3" s="54" t="s">
+      <c r="AL3" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="AM3" s="54"/>
-      <c r="AN3" s="54"/>
-      <c r="AO3" s="54"/>
-      <c r="AP3" s="54"/>
-      <c r="AQ3" s="54"/>
-      <c r="AR3" s="54"/>
-      <c r="AS3" s="54"/>
-      <c r="AT3" s="54"/>
-      <c r="AU3" s="37"/>
-      <c r="AV3" s="37"/>
-      <c r="AW3" s="37"/>
-      <c r="AX3" s="37"/>
-      <c r="AY3" s="37"/>
-      <c r="AZ3" s="37"/>
-      <c r="BA3" s="37"/>
-      <c r="BB3" s="37"/>
-      <c r="BC3" s="37"/>
-      <c r="BD3" s="37"/>
-      <c r="BE3" s="37"/>
+      <c r="AM3" s="49"/>
+      <c r="AN3" s="49"/>
+      <c r="AO3" s="49"/>
+      <c r="AP3" s="49"/>
+      <c r="AQ3" s="49"/>
+      <c r="AR3" s="49"/>
+      <c r="AS3" s="49"/>
+      <c r="AT3" s="49"/>
+      <c r="AU3" s="46" t="s">
+        <v>39</v>
+      </c>
+      <c r="AV3" s="46"/>
+      <c r="AW3" s="46"/>
+      <c r="AX3" s="46"/>
+      <c r="AY3" s="46"/>
+      <c r="AZ3" s="46"/>
+      <c r="BA3" s="46"/>
+      <c r="BB3" s="46"/>
+      <c r="BC3" s="46"/>
+      <c r="BD3" s="46"/>
+      <c r="BE3" s="46"/>
       <c r="BF3" s="29" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="3:85" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="3:85" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="4"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -1069,73 +1115,77 @@
       <c r="BE4" s="5"/>
       <c r="BF4" s="5"/>
     </row>
-    <row r="5" spans="3:85" x14ac:dyDescent="0.35">
-      <c r="C5" s="46" t="s">
+    <row r="5" spans="3:85" x14ac:dyDescent="0.25">
+      <c r="C5" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="37"/>
-      <c r="J5" s="37"/>
-      <c r="K5" s="37"/>
-      <c r="L5" s="37"/>
-      <c r="M5" s="37"/>
-      <c r="N5" s="37"/>
-      <c r="O5" s="37"/>
-      <c r="P5" s="37"/>
-      <c r="Q5" s="37"/>
-      <c r="R5" s="37"/>
-      <c r="S5" s="37"/>
-      <c r="T5" s="37"/>
-      <c r="U5" s="37"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="46" t="s">
+        <v>40</v>
+      </c>
+      <c r="J5" s="46"/>
+      <c r="K5" s="46"/>
+      <c r="L5" s="46"/>
+      <c r="M5" s="46"/>
+      <c r="N5" s="46"/>
+      <c r="O5" s="46"/>
+      <c r="P5" s="46"/>
+      <c r="Q5" s="46"/>
+      <c r="R5" s="46"/>
+      <c r="S5" s="46"/>
+      <c r="T5" s="46"/>
+      <c r="U5" s="46"/>
       <c r="V5" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="W5" s="54" t="s">
+      <c r="W5" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="X5" s="54"/>
-      <c r="Y5" s="54"/>
-      <c r="Z5" s="54"/>
-      <c r="AA5" s="54"/>
-      <c r="AB5" s="54"/>
-      <c r="AC5" s="37"/>
-      <c r="AD5" s="37"/>
-      <c r="AE5" s="37"/>
-      <c r="AF5" s="37"/>
-      <c r="AG5" s="37"/>
-      <c r="AH5" s="37"/>
-      <c r="AI5" s="37"/>
-      <c r="AJ5" s="37"/>
-      <c r="AK5" s="37"/>
-      <c r="AL5" s="37"/>
-      <c r="AM5" s="37"/>
-      <c r="AN5" s="37"/>
-      <c r="AO5" s="37"/>
-      <c r="AP5" s="37"/>
-      <c r="AQ5" s="37"/>
-      <c r="AR5" s="42" t="s">
+      <c r="X5" s="49"/>
+      <c r="Y5" s="49"/>
+      <c r="Z5" s="49"/>
+      <c r="AA5" s="49"/>
+      <c r="AB5" s="49"/>
+      <c r="AC5" s="46" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD5" s="46"/>
+      <c r="AE5" s="46"/>
+      <c r="AF5" s="46"/>
+      <c r="AG5" s="46"/>
+      <c r="AH5" s="46"/>
+      <c r="AI5" s="46"/>
+      <c r="AJ5" s="46"/>
+      <c r="AK5" s="46"/>
+      <c r="AL5" s="46"/>
+      <c r="AM5" s="46"/>
+      <c r="AN5" s="46"/>
+      <c r="AO5" s="46"/>
+      <c r="AP5" s="46"/>
+      <c r="AQ5" s="46"/>
+      <c r="AR5" s="58" t="s">
         <v>34</v>
       </c>
-      <c r="AS5" s="42"/>
-      <c r="AT5" s="42"/>
-      <c r="AU5" s="42"/>
-      <c r="AV5" s="42"/>
-      <c r="AW5" s="42"/>
-      <c r="AX5" s="42"/>
-      <c r="AY5" s="42"/>
-      <c r="AZ5" s="42"/>
-      <c r="BA5" s="42"/>
-      <c r="BB5" s="42"/>
-      <c r="BC5" s="42"/>
-      <c r="BD5" s="42"/>
-      <c r="BE5" s="42"/>
-      <c r="BF5" s="42"/>
-    </row>
-    <row r="6" spans="3:85" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AS5" s="58"/>
+      <c r="AT5" s="58"/>
+      <c r="AU5" s="58"/>
+      <c r="AV5" s="58"/>
+      <c r="AW5" s="58"/>
+      <c r="AX5" s="58"/>
+      <c r="AY5" s="58"/>
+      <c r="AZ5" s="58"/>
+      <c r="BA5" s="58"/>
+      <c r="BB5" s="58"/>
+      <c r="BC5" s="58"/>
+      <c r="BD5" s="58"/>
+      <c r="BE5" s="58"/>
+      <c r="BF5" s="58"/>
+    </row>
+    <row r="6" spans="3:85" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
@@ -1193,67 +1243,69 @@
       <c r="BE6" s="5"/>
       <c r="BF6" s="5"/>
     </row>
-    <row r="7" spans="3:85" x14ac:dyDescent="0.35">
-      <c r="C7" s="55" t="s">
+    <row r="7" spans="3:85" x14ac:dyDescent="0.25">
+      <c r="C7" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="55"/>
-      <c r="E7" s="55"/>
-      <c r="F7" s="55"/>
-      <c r="G7" s="55"/>
-      <c r="H7" s="55"/>
-      <c r="I7" s="37"/>
-      <c r="J7" s="37"/>
-      <c r="K7" s="37"/>
-      <c r="L7" s="37"/>
-      <c r="M7" s="37"/>
-      <c r="N7" s="37"/>
-      <c r="O7" s="37"/>
-      <c r="P7" s="37"/>
-      <c r="Q7" s="37"/>
-      <c r="R7" s="37"/>
-      <c r="S7" s="37"/>
-      <c r="T7" s="37"/>
-      <c r="U7" s="37"/>
-      <c r="V7" s="37"/>
-      <c r="W7" s="37"/>
-      <c r="X7" s="37"/>
-      <c r="Y7" s="37"/>
-      <c r="Z7" s="37"/>
-      <c r="AA7" s="37"/>
-      <c r="AB7" s="37"/>
-      <c r="AC7" s="37"/>
-      <c r="AD7" s="37"/>
-      <c r="AE7" s="37"/>
-      <c r="AF7" s="37"/>
-      <c r="AG7" s="37"/>
-      <c r="AH7" s="37"/>
-      <c r="AI7" s="37"/>
-      <c r="AJ7" s="37"/>
-      <c r="AK7" s="37"/>
-      <c r="AL7" s="37"/>
-      <c r="AM7" s="37"/>
-      <c r="AN7" s="37"/>
-      <c r="AO7" s="37"/>
-      <c r="AP7" s="37"/>
-      <c r="AQ7" s="37"/>
-      <c r="AR7" s="37"/>
-      <c r="AS7" s="37"/>
-      <c r="AT7" s="37"/>
-      <c r="AU7" s="37"/>
-      <c r="AV7" s="37"/>
-      <c r="AW7" s="37"/>
-      <c r="AX7" s="37"/>
-      <c r="AY7" s="37"/>
-      <c r="AZ7" s="37"/>
-      <c r="BA7" s="37"/>
-      <c r="BB7" s="37"/>
-      <c r="BC7" s="37"/>
-      <c r="BD7" s="37"/>
-      <c r="BE7" s="37"/>
-      <c r="BF7" s="37"/>
-    </row>
-    <row r="8" spans="3:85" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
+      <c r="I7" s="46" t="s">
+        <v>42</v>
+      </c>
+      <c r="J7" s="46"/>
+      <c r="K7" s="46"/>
+      <c r="L7" s="46"/>
+      <c r="M7" s="46"/>
+      <c r="N7" s="46"/>
+      <c r="O7" s="46"/>
+      <c r="P7" s="46"/>
+      <c r="Q7" s="46"/>
+      <c r="R7" s="46"/>
+      <c r="S7" s="46"/>
+      <c r="T7" s="46"/>
+      <c r="U7" s="46"/>
+      <c r="V7" s="46"/>
+      <c r="W7" s="46"/>
+      <c r="X7" s="46"/>
+      <c r="Y7" s="46"/>
+      <c r="Z7" s="46"/>
+      <c r="AA7" s="46"/>
+      <c r="AB7" s="46"/>
+      <c r="AC7" s="46"/>
+      <c r="AD7" s="46"/>
+      <c r="AE7" s="46"/>
+      <c r="AF7" s="46"/>
+      <c r="AG7" s="46"/>
+      <c r="AH7" s="46"/>
+      <c r="AI7" s="46"/>
+      <c r="AJ7" s="46"/>
+      <c r="AK7" s="46"/>
+      <c r="AL7" s="46"/>
+      <c r="AM7" s="46"/>
+      <c r="AN7" s="46"/>
+      <c r="AO7" s="46"/>
+      <c r="AP7" s="46"/>
+      <c r="AQ7" s="46"/>
+      <c r="AR7" s="46"/>
+      <c r="AS7" s="46"/>
+      <c r="AT7" s="46"/>
+      <c r="AU7" s="46"/>
+      <c r="AV7" s="46"/>
+      <c r="AW7" s="46"/>
+      <c r="AX7" s="46"/>
+      <c r="AY7" s="46"/>
+      <c r="AZ7" s="46"/>
+      <c r="BA7" s="46"/>
+      <c r="BB7" s="46"/>
+      <c r="BC7" s="46"/>
+      <c r="BD7" s="46"/>
+      <c r="BE7" s="46"/>
+      <c r="BF7" s="46"/>
+    </row>
+    <row r="8" spans="3:85" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
@@ -1311,75 +1363,79 @@
       <c r="BE8" s="4"/>
       <c r="BF8" s="6"/>
     </row>
-    <row r="9" spans="3:85" x14ac:dyDescent="0.35">
-      <c r="C9" s="46" t="s">
+    <row r="9" spans="3:85" x14ac:dyDescent="0.25">
+      <c r="C9" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="46"/>
-      <c r="G9" s="46"/>
-      <c r="H9" s="37"/>
-      <c r="I9" s="37"/>
-      <c r="J9" s="37"/>
-      <c r="K9" s="37"/>
-      <c r="L9" s="37"/>
-      <c r="M9" s="37"/>
-      <c r="N9" s="37"/>
-      <c r="O9" s="37"/>
-      <c r="P9" s="37"/>
-      <c r="Q9" s="37"/>
-      <c r="R9" s="37"/>
-      <c r="S9" s="37"/>
-      <c r="T9" s="37"/>
-      <c r="U9" s="37"/>
-      <c r="V9" s="37"/>
-      <c r="W9" s="37"/>
-      <c r="X9" s="37"/>
-      <c r="Y9" s="37"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="45"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="46" t="s">
+        <v>43</v>
+      </c>
+      <c r="I9" s="46"/>
+      <c r="J9" s="46"/>
+      <c r="K9" s="46"/>
+      <c r="L9" s="46"/>
+      <c r="M9" s="46"/>
+      <c r="N9" s="46"/>
+      <c r="O9" s="46"/>
+      <c r="P9" s="46"/>
+      <c r="Q9" s="46"/>
+      <c r="R9" s="46"/>
+      <c r="S9" s="46"/>
+      <c r="T9" s="46"/>
+      <c r="U9" s="46"/>
+      <c r="V9" s="46"/>
+      <c r="W9" s="46"/>
+      <c r="X9" s="46"/>
+      <c r="Y9" s="46"/>
       <c r="Z9" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="AA9" s="54" t="s">
+      <c r="AA9" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="AB9" s="54"/>
-      <c r="AC9" s="54"/>
-      <c r="AD9" s="54"/>
-      <c r="AE9" s="54"/>
-      <c r="AF9" s="41"/>
-      <c r="AG9" s="41"/>
-      <c r="AH9" s="41"/>
+      <c r="AB9" s="49"/>
+      <c r="AC9" s="49"/>
+      <c r="AD9" s="49"/>
+      <c r="AE9" s="49"/>
+      <c r="AF9" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG9" s="48"/>
+      <c r="AH9" s="48"/>
       <c r="AI9" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="AJ9" s="55" t="s">
+      <c r="AJ9" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="AK9" s="55"/>
-      <c r="AL9" s="55"/>
-      <c r="AM9" s="55"/>
-      <c r="AN9" s="55"/>
-      <c r="AO9" s="55"/>
-      <c r="AP9" s="55"/>
-      <c r="AQ9" s="55"/>
-      <c r="AR9" s="55"/>
-      <c r="AS9" s="55"/>
-      <c r="AT9" s="55"/>
-      <c r="AU9" s="55"/>
-      <c r="AV9" s="55"/>
-      <c r="AW9" s="55"/>
-      <c r="AX9" s="55"/>
-      <c r="AY9" s="55"/>
-      <c r="AZ9" s="55"/>
-      <c r="BA9" s="55"/>
-      <c r="BB9" s="55"/>
-      <c r="BC9" s="55"/>
-      <c r="BD9" s="55"/>
-      <c r="BE9" s="55"/>
-      <c r="BF9" s="55"/>
-    </row>
-    <row r="10" spans="3:85" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AK9" s="47"/>
+      <c r="AL9" s="47"/>
+      <c r="AM9" s="47"/>
+      <c r="AN9" s="47"/>
+      <c r="AO9" s="47"/>
+      <c r="AP9" s="47"/>
+      <c r="AQ9" s="47"/>
+      <c r="AR9" s="47"/>
+      <c r="AS9" s="47"/>
+      <c r="AT9" s="47"/>
+      <c r="AU9" s="47"/>
+      <c r="AV9" s="47"/>
+      <c r="AW9" s="47"/>
+      <c r="AX9" s="47"/>
+      <c r="AY9" s="47"/>
+      <c r="AZ9" s="47"/>
+      <c r="BA9" s="47"/>
+      <c r="BB9" s="47"/>
+      <c r="BC9" s="47"/>
+      <c r="BD9" s="47"/>
+      <c r="BE9" s="47"/>
+      <c r="BF9" s="47"/>
+    </row>
+    <row r="10" spans="3:85" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
@@ -1437,67 +1493,69 @@
       <c r="BE10" s="5"/>
       <c r="BF10" s="5"/>
     </row>
-    <row r="11" spans="3:85" x14ac:dyDescent="0.35">
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="37"/>
-      <c r="H11" s="37"/>
-      <c r="I11" s="37"/>
-      <c r="J11" s="37"/>
-      <c r="K11" s="37"/>
-      <c r="L11" s="37"/>
-      <c r="M11" s="46" t="s">
+    <row r="11" spans="3:85" x14ac:dyDescent="0.25">
+      <c r="C11" s="46" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="46"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="46"/>
+      <c r="I11" s="46"/>
+      <c r="J11" s="46"/>
+      <c r="K11" s="46"/>
+      <c r="L11" s="46"/>
+      <c r="M11" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="N11" s="46"/>
-      <c r="O11" s="46"/>
-      <c r="P11" s="46"/>
-      <c r="Q11" s="46"/>
-      <c r="R11" s="46"/>
-      <c r="S11" s="46"/>
-      <c r="T11" s="46"/>
-      <c r="U11" s="46"/>
-      <c r="V11" s="46"/>
-      <c r="W11" s="46"/>
-      <c r="X11" s="46"/>
-      <c r="Y11" s="46"/>
-      <c r="Z11" s="46"/>
-      <c r="AA11" s="46"/>
-      <c r="AB11" s="46"/>
-      <c r="AC11" s="46"/>
-      <c r="AD11" s="46"/>
-      <c r="AE11" s="46"/>
-      <c r="AF11" s="46"/>
-      <c r="AG11" s="46"/>
-      <c r="AH11" s="46"/>
-      <c r="AI11" s="46"/>
-      <c r="AJ11" s="46"/>
-      <c r="AK11" s="46"/>
-      <c r="AL11" s="46"/>
-      <c r="AM11" s="46"/>
-      <c r="AN11" s="46"/>
-      <c r="AO11" s="46"/>
-      <c r="AP11" s="46"/>
-      <c r="AQ11" s="46"/>
-      <c r="AR11" s="46"/>
-      <c r="AS11" s="46"/>
-      <c r="AT11" s="46"/>
-      <c r="AU11" s="46"/>
-      <c r="AV11" s="46"/>
-      <c r="AW11" s="46"/>
-      <c r="AX11" s="46"/>
-      <c r="AY11" s="46"/>
-      <c r="AZ11" s="46"/>
-      <c r="BA11" s="46"/>
-      <c r="BB11" s="46"/>
-      <c r="BC11" s="46"/>
-      <c r="BD11" s="46"/>
-      <c r="BE11" s="46"/>
-      <c r="BF11" s="46"/>
-    </row>
-    <row r="12" spans="3:85" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="N11" s="45"/>
+      <c r="O11" s="45"/>
+      <c r="P11" s="45"/>
+      <c r="Q11" s="45"/>
+      <c r="R11" s="45"/>
+      <c r="S11" s="45"/>
+      <c r="T11" s="45"/>
+      <c r="U11" s="45"/>
+      <c r="V11" s="45"/>
+      <c r="W11" s="45"/>
+      <c r="X11" s="45"/>
+      <c r="Y11" s="45"/>
+      <c r="Z11" s="45"/>
+      <c r="AA11" s="45"/>
+      <c r="AB11" s="45"/>
+      <c r="AC11" s="45"/>
+      <c r="AD11" s="45"/>
+      <c r="AE11" s="45"/>
+      <c r="AF11" s="45"/>
+      <c r="AG11" s="45"/>
+      <c r="AH11" s="45"/>
+      <c r="AI11" s="45"/>
+      <c r="AJ11" s="45"/>
+      <c r="AK11" s="45"/>
+      <c r="AL11" s="45"/>
+      <c r="AM11" s="45"/>
+      <c r="AN11" s="45"/>
+      <c r="AO11" s="45"/>
+      <c r="AP11" s="45"/>
+      <c r="AQ11" s="45"/>
+      <c r="AR11" s="45"/>
+      <c r="AS11" s="45"/>
+      <c r="AT11" s="45"/>
+      <c r="AU11" s="45"/>
+      <c r="AV11" s="45"/>
+      <c r="AW11" s="45"/>
+      <c r="AX11" s="45"/>
+      <c r="AY11" s="45"/>
+      <c r="AZ11" s="45"/>
+      <c r="BA11" s="45"/>
+      <c r="BB11" s="45"/>
+      <c r="BC11" s="45"/>
+      <c r="BD11" s="45"/>
+      <c r="BE11" s="45"/>
+      <c r="BF11" s="45"/>
+    </row>
+    <row r="12" spans="3:85" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
@@ -1555,133 +1613,135 @@
       <c r="BE12" s="5"/>
       <c r="BF12" s="5"/>
     </row>
-    <row r="13" spans="3:85" s="22" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C13" s="56"/>
-      <c r="D13" s="56"/>
-      <c r="E13" s="56"/>
-      <c r="F13" s="56"/>
-      <c r="G13" s="56"/>
-      <c r="H13" s="56"/>
-      <c r="I13" s="56"/>
-      <c r="J13" s="56"/>
-      <c r="K13" s="56"/>
-      <c r="L13" s="56"/>
-      <c r="M13" s="56"/>
-      <c r="N13" s="56"/>
-      <c r="O13" s="56"/>
-      <c r="P13" s="56"/>
-      <c r="Q13" s="56"/>
-      <c r="R13" s="56"/>
-      <c r="S13" s="56"/>
-      <c r="T13" s="56"/>
-      <c r="U13" s="56"/>
-      <c r="V13" s="56"/>
-      <c r="W13" s="56"/>
-      <c r="X13" s="56"/>
-      <c r="Y13" s="56"/>
-      <c r="Z13" s="56"/>
-      <c r="AA13" s="56"/>
-      <c r="AB13" s="56"/>
-      <c r="AC13" s="56"/>
-      <c r="AD13" s="56"/>
-      <c r="AE13" s="56"/>
-      <c r="AF13" s="56"/>
-      <c r="AG13" s="56"/>
-      <c r="AH13" s="56"/>
-      <c r="AI13" s="56"/>
-      <c r="AJ13" s="56"/>
-      <c r="AK13" s="56"/>
-      <c r="AL13" s="56"/>
-      <c r="AM13" s="56"/>
-      <c r="AN13" s="56"/>
-      <c r="AO13" s="56"/>
-      <c r="AP13" s="56"/>
-      <c r="AQ13" s="56"/>
-      <c r="AR13" s="56"/>
-      <c r="AS13" s="56"/>
-      <c r="AT13" s="56"/>
-      <c r="AU13" s="56"/>
-      <c r="AV13" s="56"/>
-      <c r="AW13" s="56"/>
-      <c r="AX13" s="56"/>
-      <c r="AY13" s="56"/>
-      <c r="AZ13" s="56"/>
-      <c r="BA13" s="56"/>
-      <c r="BB13" s="56"/>
-      <c r="BC13" s="56"/>
-      <c r="BD13" s="56"/>
-      <c r="BE13" s="56"/>
-      <c r="BF13" s="56"/>
-      <c r="BI13" s="36"/>
-      <c r="BJ13" s="36"/>
+    <row r="13" spans="3:85" s="22" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C13" s="57" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="57"/>
+      <c r="E13" s="57"/>
+      <c r="F13" s="57"/>
+      <c r="G13" s="57"/>
+      <c r="H13" s="57"/>
+      <c r="I13" s="57"/>
+      <c r="J13" s="57"/>
+      <c r="K13" s="57"/>
+      <c r="L13" s="57"/>
+      <c r="M13" s="57"/>
+      <c r="N13" s="57"/>
+      <c r="O13" s="57"/>
+      <c r="P13" s="57"/>
+      <c r="Q13" s="57"/>
+      <c r="R13" s="57"/>
+      <c r="S13" s="57"/>
+      <c r="T13" s="57"/>
+      <c r="U13" s="57"/>
+      <c r="V13" s="57"/>
+      <c r="W13" s="57"/>
+      <c r="X13" s="57"/>
+      <c r="Y13" s="57"/>
+      <c r="Z13" s="57"/>
+      <c r="AA13" s="57"/>
+      <c r="AB13" s="57"/>
+      <c r="AC13" s="57"/>
+      <c r="AD13" s="57"/>
+      <c r="AE13" s="57"/>
+      <c r="AF13" s="57"/>
+      <c r="AG13" s="57"/>
+      <c r="AH13" s="57"/>
+      <c r="AI13" s="57"/>
+      <c r="AJ13" s="57"/>
+      <c r="AK13" s="57"/>
+      <c r="AL13" s="57"/>
+      <c r="AM13" s="57"/>
+      <c r="AN13" s="57"/>
+      <c r="AO13" s="57"/>
+      <c r="AP13" s="57"/>
+      <c r="AQ13" s="57"/>
+      <c r="AR13" s="57"/>
+      <c r="AS13" s="57"/>
+      <c r="AT13" s="57"/>
+      <c r="AU13" s="57"/>
+      <c r="AV13" s="57"/>
+      <c r="AW13" s="57"/>
+      <c r="AX13" s="57"/>
+      <c r="AY13" s="57"/>
+      <c r="AZ13" s="57"/>
+      <c r="BA13" s="57"/>
+      <c r="BB13" s="57"/>
+      <c r="BC13" s="57"/>
+      <c r="BD13" s="57"/>
+      <c r="BE13" s="57"/>
+      <c r="BF13" s="57"/>
+      <c r="BI13" s="62"/>
+      <c r="BJ13" s="62"/>
       <c r="BK13" s="26"/>
       <c r="BM13" s="24"/>
       <c r="CG13" s="23"/>
     </row>
-    <row r="14" spans="3:85" s="22" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C14" s="38"/>
-      <c r="D14" s="38"/>
-      <c r="E14" s="38"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="38"/>
-      <c r="I14" s="38"/>
-      <c r="J14" s="38"/>
-      <c r="K14" s="38"/>
-      <c r="L14" s="38"/>
-      <c r="M14" s="38"/>
-      <c r="N14" s="38"/>
-      <c r="O14" s="38"/>
-      <c r="P14" s="38"/>
-      <c r="Q14" s="38"/>
-      <c r="R14" s="38"/>
-      <c r="S14" s="38"/>
-      <c r="T14" s="38"/>
-      <c r="U14" s="38"/>
-      <c r="V14" s="38"/>
-      <c r="W14" s="38"/>
-      <c r="X14" s="38"/>
-      <c r="Y14" s="38"/>
-      <c r="Z14" s="38"/>
-      <c r="AA14" s="38"/>
-      <c r="AB14" s="38"/>
-      <c r="AC14" s="38"/>
-      <c r="AD14" s="38"/>
-      <c r="AE14" s="38"/>
-      <c r="AF14" s="38"/>
-      <c r="AG14" s="38"/>
-      <c r="AH14" s="38"/>
-      <c r="AI14" s="38"/>
-      <c r="AJ14" s="38"/>
-      <c r="AK14" s="38"/>
-      <c r="AL14" s="38"/>
-      <c r="AM14" s="38"/>
-      <c r="AN14" s="38"/>
-      <c r="AO14" s="38"/>
-      <c r="AP14" s="38"/>
-      <c r="AQ14" s="38"/>
-      <c r="AR14" s="38"/>
-      <c r="AS14" s="38"/>
-      <c r="AT14" s="38"/>
-      <c r="AU14" s="38"/>
-      <c r="AV14" s="38"/>
-      <c r="AW14" s="38"/>
-      <c r="AX14" s="38"/>
-      <c r="AY14" s="38"/>
-      <c r="AZ14" s="38"/>
-      <c r="BA14" s="38"/>
-      <c r="BB14" s="38"/>
-      <c r="BC14" s="38"/>
-      <c r="BD14" s="38"/>
-      <c r="BE14" s="38"/>
-      <c r="BF14" s="38"/>
+    <row r="14" spans="3:85" s="22" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="63"/>
+      <c r="D14" s="63"/>
+      <c r="E14" s="63"/>
+      <c r="F14" s="63"/>
+      <c r="G14" s="63"/>
+      <c r="H14" s="63"/>
+      <c r="I14" s="63"/>
+      <c r="J14" s="63"/>
+      <c r="K14" s="63"/>
+      <c r="L14" s="63"/>
+      <c r="M14" s="63"/>
+      <c r="N14" s="63"/>
+      <c r="O14" s="63"/>
+      <c r="P14" s="63"/>
+      <c r="Q14" s="63"/>
+      <c r="R14" s="63"/>
+      <c r="S14" s="63"/>
+      <c r="T14" s="63"/>
+      <c r="U14" s="63"/>
+      <c r="V14" s="63"/>
+      <c r="W14" s="63"/>
+      <c r="X14" s="63"/>
+      <c r="Y14" s="63"/>
+      <c r="Z14" s="63"/>
+      <c r="AA14" s="63"/>
+      <c r="AB14" s="63"/>
+      <c r="AC14" s="63"/>
+      <c r="AD14" s="63"/>
+      <c r="AE14" s="63"/>
+      <c r="AF14" s="63"/>
+      <c r="AG14" s="63"/>
+      <c r="AH14" s="63"/>
+      <c r="AI14" s="63"/>
+      <c r="AJ14" s="63"/>
+      <c r="AK14" s="63"/>
+      <c r="AL14" s="63"/>
+      <c r="AM14" s="63"/>
+      <c r="AN14" s="63"/>
+      <c r="AO14" s="63"/>
+      <c r="AP14" s="63"/>
+      <c r="AQ14" s="63"/>
+      <c r="AR14" s="63"/>
+      <c r="AS14" s="63"/>
+      <c r="AT14" s="63"/>
+      <c r="AU14" s="63"/>
+      <c r="AV14" s="63"/>
+      <c r="AW14" s="63"/>
+      <c r="AX14" s="63"/>
+      <c r="AY14" s="63"/>
+      <c r="AZ14" s="63"/>
+      <c r="BA14" s="63"/>
+      <c r="BB14" s="63"/>
+      <c r="BC14" s="63"/>
+      <c r="BD14" s="63"/>
+      <c r="BE14" s="63"/>
+      <c r="BF14" s="63"/>
       <c r="BI14" s="25"/>
       <c r="BJ14" s="25"/>
       <c r="BK14" s="26"/>
       <c r="BM14" s="24"/>
       <c r="CG14" s="23"/>
     </row>
-    <row r="15" spans="3:85" x14ac:dyDescent="0.35">
+    <row r="15" spans="3:85" x14ac:dyDescent="0.25">
       <c r="C15" s="5" t="s">
         <v>22</v>
       </c>
@@ -1702,55 +1762,57 @@
       <c r="P15" s="4"/>
       <c r="Q15" s="4"/>
       <c r="R15" s="4"/>
-      <c r="S15" s="37"/>
-      <c r="T15" s="37"/>
-      <c r="U15" s="37"/>
-      <c r="V15" s="37"/>
-      <c r="W15" s="37"/>
-      <c r="X15" s="37"/>
-      <c r="Y15" s="37"/>
-      <c r="Z15" s="37"/>
-      <c r="AA15" s="37"/>
-      <c r="AB15" s="37"/>
-      <c r="AC15" s="39" t="s">
+      <c r="S15" s="46" t="s">
+        <v>47</v>
+      </c>
+      <c r="T15" s="46"/>
+      <c r="U15" s="46"/>
+      <c r="V15" s="46"/>
+      <c r="W15" s="46"/>
+      <c r="X15" s="46"/>
+      <c r="Y15" s="46"/>
+      <c r="Z15" s="46"/>
+      <c r="AA15" s="46"/>
+      <c r="AB15" s="46"/>
+      <c r="AC15" s="64" t="s">
         <v>36</v>
       </c>
-      <c r="AD15" s="39"/>
-      <c r="AE15" s="39"/>
-      <c r="AF15" s="39"/>
-      <c r="AG15" s="39"/>
-      <c r="AH15" s="39"/>
-      <c r="AI15" s="39"/>
-      <c r="AJ15" s="39"/>
-      <c r="AK15" s="39"/>
-      <c r="AL15" s="39"/>
-      <c r="AM15" s="39"/>
-      <c r="AN15" s="39"/>
-      <c r="AO15" s="39"/>
-      <c r="AP15" s="39"/>
-      <c r="AQ15" s="39"/>
-      <c r="AR15" s="39"/>
-      <c r="AS15" s="39"/>
-      <c r="AT15" s="39"/>
-      <c r="AU15" s="39"/>
-      <c r="AV15" s="39"/>
-      <c r="AW15" s="39"/>
-      <c r="AX15" s="39"/>
-      <c r="AY15" s="39"/>
-      <c r="AZ15" s="39"/>
-      <c r="BA15" s="39"/>
-      <c r="BB15" s="39"/>
-      <c r="BC15" s="39"/>
-      <c r="BD15" s="39"/>
-      <c r="BE15" s="39"/>
-      <c r="BF15" s="39"/>
+      <c r="AD15" s="64"/>
+      <c r="AE15" s="64"/>
+      <c r="AF15" s="64"/>
+      <c r="AG15" s="64"/>
+      <c r="AH15" s="64"/>
+      <c r="AI15" s="64"/>
+      <c r="AJ15" s="64"/>
+      <c r="AK15" s="64"/>
+      <c r="AL15" s="64"/>
+      <c r="AM15" s="64"/>
+      <c r="AN15" s="64"/>
+      <c r="AO15" s="64"/>
+      <c r="AP15" s="64"/>
+      <c r="AQ15" s="64"/>
+      <c r="AR15" s="64"/>
+      <c r="AS15" s="64"/>
+      <c r="AT15" s="64"/>
+      <c r="AU15" s="64"/>
+      <c r="AV15" s="64"/>
+      <c r="AW15" s="64"/>
+      <c r="AX15" s="64"/>
+      <c r="AY15" s="64"/>
+      <c r="AZ15" s="64"/>
+      <c r="BA15" s="64"/>
+      <c r="BB15" s="64"/>
+      <c r="BC15" s="64"/>
+      <c r="BD15" s="64"/>
+      <c r="BE15" s="64"/>
+      <c r="BF15" s="64"/>
       <c r="BH15" s="22"/>
       <c r="BJ15" s="22"/>
       <c r="BL15" s="23"/>
       <c r="BX15" s="22"/>
       <c r="BY15" s="22"/>
     </row>
-    <row r="16" spans="3:85" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="3:85" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
@@ -1808,7 +1870,7 @@
       <c r="BE16" s="5"/>
       <c r="BF16" s="5"/>
     </row>
-    <row r="17" spans="3:58" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:58" x14ac:dyDescent="0.25">
       <c r="C17" s="27" t="s">
         <v>37</v>
       </c>
@@ -1817,20 +1879,26 @@
       <c r="F17" s="31"/>
       <c r="G17" s="31"/>
       <c r="H17" s="31"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
+      <c r="I17" s="65" t="s">
+        <v>48</v>
+      </c>
+      <c r="J17" s="65"/>
       <c r="K17" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="L17" s="41"/>
-      <c r="M17" s="41"/>
+      <c r="L17" s="48">
+        <v>2</v>
+      </c>
+      <c r="M17" s="48"/>
       <c r="N17" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="O17" s="41"/>
-      <c r="P17" s="41"/>
-      <c r="Q17" s="41"/>
-      <c r="R17" s="41"/>
+      <c r="O17" s="48">
+        <v>2018</v>
+      </c>
+      <c r="P17" s="48"/>
+      <c r="Q17" s="48"/>
+      <c r="R17" s="48"/>
       <c r="S17" s="32" t="s">
         <v>21</v>
       </c>
@@ -1862,19 +1930,19 @@
       <c r="AS17" s="32"/>
       <c r="AT17" s="32"/>
       <c r="AU17" s="32"/>
-      <c r="AV17" s="44"/>
-      <c r="AW17" s="44"/>
+      <c r="AV17" s="60"/>
+      <c r="AW17" s="60"/>
       <c r="AX17" s="33"/>
-      <c r="AY17" s="45"/>
-      <c r="AZ17" s="45"/>
+      <c r="AY17" s="61"/>
+      <c r="AZ17" s="61"/>
       <c r="BA17" s="34"/>
-      <c r="BB17" s="45"/>
-      <c r="BC17" s="45"/>
-      <c r="BD17" s="45"/>
-      <c r="BE17" s="45"/>
+      <c r="BB17" s="61"/>
+      <c r="BC17" s="61"/>
+      <c r="BD17" s="61"/>
+      <c r="BE17" s="61"/>
       <c r="BF17" s="28"/>
     </row>
-    <row r="18" spans="3:58" ht="12.9" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:58" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" s="35"/>
       <c r="D18" s="35"/>
       <c r="E18" s="35"/>
@@ -1932,189 +2000,191 @@
       <c r="BE18" s="35"/>
       <c r="BF18" s="35"/>
     </row>
-    <row r="19" spans="3:58" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C19" s="58" t="s">
+    <row r="19" spans="3:58" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="58"/>
+      <c r="D19" s="37"/>
       <c r="E19" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="F19" s="21"/>
+      <c r="F19" s="21" t="s">
+        <v>49</v>
+      </c>
       <c r="G19" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H19" s="59" t="s">
+      <c r="H19" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="I19" s="59"/>
-      <c r="J19" s="59"/>
-      <c r="K19" s="59"/>
-      <c r="L19" s="59"/>
-      <c r="M19" s="59"/>
-      <c r="N19" s="59"/>
-      <c r="O19" s="59"/>
-      <c r="P19" s="59"/>
-      <c r="Q19" s="59"/>
-      <c r="R19" s="59"/>
-      <c r="S19" s="59"/>
-      <c r="T19" s="59"/>
-      <c r="U19" s="59"/>
-      <c r="V19" s="59"/>
-      <c r="W19" s="59"/>
-      <c r="X19" s="59"/>
-      <c r="Y19" s="59"/>
-      <c r="Z19" s="59"/>
-      <c r="AA19" s="59"/>
-      <c r="AB19" s="59"/>
-      <c r="AC19" s="59"/>
-      <c r="AD19" s="59"/>
-      <c r="AE19" s="59"/>
-      <c r="AF19" s="59"/>
-      <c r="AG19" s="59"/>
-      <c r="AH19" s="59"/>
-      <c r="AI19" s="59"/>
-      <c r="AJ19" s="59"/>
-      <c r="AK19" s="59"/>
-      <c r="AL19" s="59"/>
-      <c r="AM19" s="59"/>
-      <c r="AN19" s="59"/>
-      <c r="AO19" s="59"/>
-      <c r="AP19" s="59"/>
-      <c r="AQ19" s="59"/>
-      <c r="AR19" s="59"/>
-      <c r="AS19" s="59"/>
-      <c r="AT19" s="59"/>
-      <c r="AU19" s="59"/>
-      <c r="AV19" s="59"/>
-      <c r="AW19" s="59"/>
-      <c r="AX19" s="59"/>
-      <c r="AY19" s="59"/>
-      <c r="AZ19" s="59"/>
-      <c r="BA19" s="59"/>
-      <c r="BB19" s="59"/>
-      <c r="BC19" s="59"/>
-      <c r="BD19" s="59"/>
-      <c r="BE19" s="59"/>
-      <c r="BF19" s="59"/>
-    </row>
-    <row r="20" spans="3:58" x14ac:dyDescent="0.35">
+      <c r="I19" s="38"/>
+      <c r="J19" s="38"/>
+      <c r="K19" s="38"/>
+      <c r="L19" s="38"/>
+      <c r="M19" s="38"/>
+      <c r="N19" s="38"/>
+      <c r="O19" s="38"/>
+      <c r="P19" s="38"/>
+      <c r="Q19" s="38"/>
+      <c r="R19" s="38"/>
+      <c r="S19" s="38"/>
+      <c r="T19" s="38"/>
+      <c r="U19" s="38"/>
+      <c r="V19" s="38"/>
+      <c r="W19" s="38"/>
+      <c r="X19" s="38"/>
+      <c r="Y19" s="38"/>
+      <c r="Z19" s="38"/>
+      <c r="AA19" s="38"/>
+      <c r="AB19" s="38"/>
+      <c r="AC19" s="38"/>
+      <c r="AD19" s="38"/>
+      <c r="AE19" s="38"/>
+      <c r="AF19" s="38"/>
+      <c r="AG19" s="38"/>
+      <c r="AH19" s="38"/>
+      <c r="AI19" s="38"/>
+      <c r="AJ19" s="38"/>
+      <c r="AK19" s="38"/>
+      <c r="AL19" s="38"/>
+      <c r="AM19" s="38"/>
+      <c r="AN19" s="38"/>
+      <c r="AO19" s="38"/>
+      <c r="AP19" s="38"/>
+      <c r="AQ19" s="38"/>
+      <c r="AR19" s="38"/>
+      <c r="AS19" s="38"/>
+      <c r="AT19" s="38"/>
+      <c r="AU19" s="38"/>
+      <c r="AV19" s="38"/>
+      <c r="AW19" s="38"/>
+      <c r="AX19" s="38"/>
+      <c r="AY19" s="38"/>
+      <c r="AZ19" s="38"/>
+      <c r="BA19" s="38"/>
+      <c r="BB19" s="38"/>
+      <c r="BC19" s="38"/>
+      <c r="BD19" s="38"/>
+      <c r="BE19" s="38"/>
+      <c r="BF19" s="38"/>
+    </row>
+    <row r="20" spans="3:58" x14ac:dyDescent="0.25">
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
-      <c r="H20" s="59"/>
-      <c r="I20" s="59"/>
-      <c r="J20" s="59"/>
-      <c r="K20" s="59"/>
-      <c r="L20" s="59"/>
-      <c r="M20" s="59"/>
-      <c r="N20" s="59"/>
-      <c r="O20" s="59"/>
-      <c r="P20" s="59"/>
-      <c r="Q20" s="59"/>
-      <c r="R20" s="59"/>
-      <c r="S20" s="59"/>
-      <c r="T20" s="59"/>
-      <c r="U20" s="59"/>
-      <c r="V20" s="59"/>
-      <c r="W20" s="59"/>
-      <c r="X20" s="59"/>
-      <c r="Y20" s="59"/>
-      <c r="Z20" s="59"/>
-      <c r="AA20" s="59"/>
-      <c r="AB20" s="59"/>
-      <c r="AC20" s="59"/>
-      <c r="AD20" s="59"/>
-      <c r="AE20" s="59"/>
-      <c r="AF20" s="59"/>
-      <c r="AG20" s="59"/>
-      <c r="AH20" s="59"/>
-      <c r="AI20" s="59"/>
-      <c r="AJ20" s="59"/>
-      <c r="AK20" s="59"/>
-      <c r="AL20" s="59"/>
-      <c r="AM20" s="59"/>
-      <c r="AN20" s="59"/>
-      <c r="AO20" s="59"/>
-      <c r="AP20" s="59"/>
-      <c r="AQ20" s="59"/>
-      <c r="AR20" s="59"/>
-      <c r="AS20" s="59"/>
-      <c r="AT20" s="59"/>
-      <c r="AU20" s="59"/>
-      <c r="AV20" s="59"/>
-      <c r="AW20" s="59"/>
-      <c r="AX20" s="59"/>
-      <c r="AY20" s="59"/>
-      <c r="AZ20" s="59"/>
-      <c r="BA20" s="59"/>
-      <c r="BB20" s="59"/>
-      <c r="BC20" s="59"/>
-      <c r="BD20" s="59"/>
-      <c r="BE20" s="59"/>
-      <c r="BF20" s="59"/>
-    </row>
-    <row r="21" spans="3:58" x14ac:dyDescent="0.35">
+      <c r="H20" s="38"/>
+      <c r="I20" s="38"/>
+      <c r="J20" s="38"/>
+      <c r="K20" s="38"/>
+      <c r="L20" s="38"/>
+      <c r="M20" s="38"/>
+      <c r="N20" s="38"/>
+      <c r="O20" s="38"/>
+      <c r="P20" s="38"/>
+      <c r="Q20" s="38"/>
+      <c r="R20" s="38"/>
+      <c r="S20" s="38"/>
+      <c r="T20" s="38"/>
+      <c r="U20" s="38"/>
+      <c r="V20" s="38"/>
+      <c r="W20" s="38"/>
+      <c r="X20" s="38"/>
+      <c r="Y20" s="38"/>
+      <c r="Z20" s="38"/>
+      <c r="AA20" s="38"/>
+      <c r="AB20" s="38"/>
+      <c r="AC20" s="38"/>
+      <c r="AD20" s="38"/>
+      <c r="AE20" s="38"/>
+      <c r="AF20" s="38"/>
+      <c r="AG20" s="38"/>
+      <c r="AH20" s="38"/>
+      <c r="AI20" s="38"/>
+      <c r="AJ20" s="38"/>
+      <c r="AK20" s="38"/>
+      <c r="AL20" s="38"/>
+      <c r="AM20" s="38"/>
+      <c r="AN20" s="38"/>
+      <c r="AO20" s="38"/>
+      <c r="AP20" s="38"/>
+      <c r="AQ20" s="38"/>
+      <c r="AR20" s="38"/>
+      <c r="AS20" s="38"/>
+      <c r="AT20" s="38"/>
+      <c r="AU20" s="38"/>
+      <c r="AV20" s="38"/>
+      <c r="AW20" s="38"/>
+      <c r="AX20" s="38"/>
+      <c r="AY20" s="38"/>
+      <c r="AZ20" s="38"/>
+      <c r="BA20" s="38"/>
+      <c r="BB20" s="38"/>
+      <c r="BC20" s="38"/>
+      <c r="BD20" s="38"/>
+      <c r="BE20" s="38"/>
+      <c r="BF20" s="38"/>
+    </row>
+    <row r="21" spans="3:58" x14ac:dyDescent="0.25">
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
-      <c r="H21" s="59"/>
-      <c r="I21" s="59"/>
-      <c r="J21" s="59"/>
-      <c r="K21" s="59"/>
-      <c r="L21" s="59"/>
-      <c r="M21" s="59"/>
-      <c r="N21" s="59"/>
-      <c r="O21" s="59"/>
-      <c r="P21" s="59"/>
-      <c r="Q21" s="59"/>
-      <c r="R21" s="59"/>
-      <c r="S21" s="59"/>
-      <c r="T21" s="59"/>
-      <c r="U21" s="59"/>
-      <c r="V21" s="59"/>
-      <c r="W21" s="59"/>
-      <c r="X21" s="59"/>
-      <c r="Y21" s="59"/>
-      <c r="Z21" s="59"/>
-      <c r="AA21" s="59"/>
-      <c r="AB21" s="59"/>
-      <c r="AC21" s="59"/>
-      <c r="AD21" s="59"/>
-      <c r="AE21" s="59"/>
-      <c r="AF21" s="59"/>
-      <c r="AG21" s="59"/>
-      <c r="AH21" s="59"/>
-      <c r="AI21" s="59"/>
-      <c r="AJ21" s="59"/>
-      <c r="AK21" s="59"/>
-      <c r="AL21" s="59"/>
-      <c r="AM21" s="59"/>
-      <c r="AN21" s="59"/>
-      <c r="AO21" s="59"/>
-      <c r="AP21" s="59"/>
-      <c r="AQ21" s="59"/>
-      <c r="AR21" s="59"/>
-      <c r="AS21" s="59"/>
-      <c r="AT21" s="59"/>
-      <c r="AU21" s="59"/>
-      <c r="AV21" s="59"/>
-      <c r="AW21" s="59"/>
-      <c r="AX21" s="59"/>
-      <c r="AY21" s="59"/>
-      <c r="AZ21" s="59"/>
-      <c r="BA21" s="59"/>
-      <c r="BB21" s="59"/>
-      <c r="BC21" s="59"/>
-      <c r="BD21" s="59"/>
-      <c r="BE21" s="59"/>
-      <c r="BF21" s="59"/>
-    </row>
-    <row r="22" spans="3:58" ht="12.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H21" s="38"/>
+      <c r="I21" s="38"/>
+      <c r="J21" s="38"/>
+      <c r="K21" s="38"/>
+      <c r="L21" s="38"/>
+      <c r="M21" s="38"/>
+      <c r="N21" s="38"/>
+      <c r="O21" s="38"/>
+      <c r="P21" s="38"/>
+      <c r="Q21" s="38"/>
+      <c r="R21" s="38"/>
+      <c r="S21" s="38"/>
+      <c r="T21" s="38"/>
+      <c r="U21" s="38"/>
+      <c r="V21" s="38"/>
+      <c r="W21" s="38"/>
+      <c r="X21" s="38"/>
+      <c r="Y21" s="38"/>
+      <c r="Z21" s="38"/>
+      <c r="AA21" s="38"/>
+      <c r="AB21" s="38"/>
+      <c r="AC21" s="38"/>
+      <c r="AD21" s="38"/>
+      <c r="AE21" s="38"/>
+      <c r="AF21" s="38"/>
+      <c r="AG21" s="38"/>
+      <c r="AH21" s="38"/>
+      <c r="AI21" s="38"/>
+      <c r="AJ21" s="38"/>
+      <c r="AK21" s="38"/>
+      <c r="AL21" s="38"/>
+      <c r="AM21" s="38"/>
+      <c r="AN21" s="38"/>
+      <c r="AO21" s="38"/>
+      <c r="AP21" s="38"/>
+      <c r="AQ21" s="38"/>
+      <c r="AR21" s="38"/>
+      <c r="AS21" s="38"/>
+      <c r="AT21" s="38"/>
+      <c r="AU21" s="38"/>
+      <c r="AV21" s="38"/>
+      <c r="AW21" s="38"/>
+      <c r="AX21" s="38"/>
+      <c r="AY21" s="38"/>
+      <c r="AZ21" s="38"/>
+      <c r="BA21" s="38"/>
+      <c r="BB21" s="38"/>
+      <c r="BC21" s="38"/>
+      <c r="BD21" s="38"/>
+      <c r="BE21" s="38"/>
+      <c r="BF21" s="38"/>
+    </row>
+    <row r="22" spans="3:58" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -2172,11 +2242,11 @@
       <c r="BE22" s="12"/>
       <c r="BF22" s="12"/>
     </row>
-    <row r="23" spans="3:58" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C23" s="58" t="s">
+    <row r="23" spans="3:58" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C23" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="D23" s="58"/>
+      <c r="D23" s="37"/>
       <c r="E23" s="11" t="s">
         <v>10</v>
       </c>
@@ -2184,235 +2254,235 @@
       <c r="G23" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H23" s="59" t="s">
+      <c r="H23" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="I23" s="59"/>
-      <c r="J23" s="59"/>
-      <c r="K23" s="59"/>
-      <c r="L23" s="59"/>
-      <c r="M23" s="59"/>
-      <c r="N23" s="59"/>
-      <c r="O23" s="59"/>
-      <c r="P23" s="59"/>
-      <c r="Q23" s="59"/>
-      <c r="R23" s="59"/>
-      <c r="S23" s="59"/>
-      <c r="T23" s="59"/>
-      <c r="U23" s="59"/>
-      <c r="V23" s="59"/>
-      <c r="W23" s="59"/>
-      <c r="X23" s="59"/>
-      <c r="Y23" s="59"/>
-      <c r="Z23" s="59"/>
-      <c r="AA23" s="59"/>
-      <c r="AB23" s="59"/>
-      <c r="AC23" s="59"/>
-      <c r="AD23" s="59"/>
-      <c r="AE23" s="59"/>
-      <c r="AF23" s="59"/>
-      <c r="AG23" s="59"/>
-      <c r="AH23" s="59"/>
-      <c r="AI23" s="59"/>
-      <c r="AJ23" s="59"/>
-      <c r="AK23" s="59"/>
-      <c r="AL23" s="59"/>
-      <c r="AM23" s="59"/>
-      <c r="AN23" s="59"/>
-      <c r="AO23" s="59"/>
-      <c r="AP23" s="59"/>
-      <c r="AQ23" s="59"/>
-      <c r="AR23" s="59"/>
-      <c r="AS23" s="59"/>
-      <c r="AT23" s="59"/>
-      <c r="AU23" s="59"/>
-      <c r="AV23" s="59"/>
-      <c r="AW23" s="59"/>
-      <c r="AX23" s="59"/>
-      <c r="AY23" s="59"/>
-      <c r="AZ23" s="59"/>
-      <c r="BA23" s="59"/>
-      <c r="BB23" s="59"/>
-      <c r="BC23" s="59"/>
-      <c r="BD23" s="59"/>
-      <c r="BE23" s="59"/>
-      <c r="BF23" s="59"/>
-    </row>
-    <row r="24" spans="3:58" x14ac:dyDescent="0.35">
+      <c r="I23" s="38"/>
+      <c r="J23" s="38"/>
+      <c r="K23" s="38"/>
+      <c r="L23" s="38"/>
+      <c r="M23" s="38"/>
+      <c r="N23" s="38"/>
+      <c r="O23" s="38"/>
+      <c r="P23" s="38"/>
+      <c r="Q23" s="38"/>
+      <c r="R23" s="38"/>
+      <c r="S23" s="38"/>
+      <c r="T23" s="38"/>
+      <c r="U23" s="38"/>
+      <c r="V23" s="38"/>
+      <c r="W23" s="38"/>
+      <c r="X23" s="38"/>
+      <c r="Y23" s="38"/>
+      <c r="Z23" s="38"/>
+      <c r="AA23" s="38"/>
+      <c r="AB23" s="38"/>
+      <c r="AC23" s="38"/>
+      <c r="AD23" s="38"/>
+      <c r="AE23" s="38"/>
+      <c r="AF23" s="38"/>
+      <c r="AG23" s="38"/>
+      <c r="AH23" s="38"/>
+      <c r="AI23" s="38"/>
+      <c r="AJ23" s="38"/>
+      <c r="AK23" s="38"/>
+      <c r="AL23" s="38"/>
+      <c r="AM23" s="38"/>
+      <c r="AN23" s="38"/>
+      <c r="AO23" s="38"/>
+      <c r="AP23" s="38"/>
+      <c r="AQ23" s="38"/>
+      <c r="AR23" s="38"/>
+      <c r="AS23" s="38"/>
+      <c r="AT23" s="38"/>
+      <c r="AU23" s="38"/>
+      <c r="AV23" s="38"/>
+      <c r="AW23" s="38"/>
+      <c r="AX23" s="38"/>
+      <c r="AY23" s="38"/>
+      <c r="AZ23" s="38"/>
+      <c r="BA23" s="38"/>
+      <c r="BB23" s="38"/>
+      <c r="BC23" s="38"/>
+      <c r="BD23" s="38"/>
+      <c r="BE23" s="38"/>
+      <c r="BF23" s="38"/>
+    </row>
+    <row r="24" spans="3:58" x14ac:dyDescent="0.25">
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
-      <c r="H24" s="59"/>
-      <c r="I24" s="59"/>
-      <c r="J24" s="59"/>
-      <c r="K24" s="59"/>
-      <c r="L24" s="59"/>
-      <c r="M24" s="59"/>
-      <c r="N24" s="59"/>
-      <c r="O24" s="59"/>
-      <c r="P24" s="59"/>
-      <c r="Q24" s="59"/>
-      <c r="R24" s="59"/>
-      <c r="S24" s="59"/>
-      <c r="T24" s="59"/>
-      <c r="U24" s="59"/>
-      <c r="V24" s="59"/>
-      <c r="W24" s="59"/>
-      <c r="X24" s="59"/>
-      <c r="Y24" s="59"/>
-      <c r="Z24" s="59"/>
-      <c r="AA24" s="59"/>
-      <c r="AB24" s="59"/>
-      <c r="AC24" s="59"/>
-      <c r="AD24" s="59"/>
-      <c r="AE24" s="59"/>
-      <c r="AF24" s="59"/>
-      <c r="AG24" s="59"/>
-      <c r="AH24" s="59"/>
-      <c r="AI24" s="59"/>
-      <c r="AJ24" s="59"/>
-      <c r="AK24" s="59"/>
-      <c r="AL24" s="59"/>
-      <c r="AM24" s="59"/>
-      <c r="AN24" s="59"/>
-      <c r="AO24" s="59"/>
-      <c r="AP24" s="59"/>
-      <c r="AQ24" s="59"/>
-      <c r="AR24" s="59"/>
-      <c r="AS24" s="59"/>
-      <c r="AT24" s="59"/>
-      <c r="AU24" s="59"/>
-      <c r="AV24" s="59"/>
-      <c r="AW24" s="59"/>
-      <c r="AX24" s="59"/>
-      <c r="AY24" s="59"/>
-      <c r="AZ24" s="59"/>
-      <c r="BA24" s="59"/>
-      <c r="BB24" s="59"/>
-      <c r="BC24" s="59"/>
-      <c r="BD24" s="59"/>
-      <c r="BE24" s="59"/>
-      <c r="BF24" s="59"/>
-    </row>
-    <row r="25" spans="3:58" x14ac:dyDescent="0.35">
+      <c r="H24" s="38"/>
+      <c r="I24" s="38"/>
+      <c r="J24" s="38"/>
+      <c r="K24" s="38"/>
+      <c r="L24" s="38"/>
+      <c r="M24" s="38"/>
+      <c r="N24" s="38"/>
+      <c r="O24" s="38"/>
+      <c r="P24" s="38"/>
+      <c r="Q24" s="38"/>
+      <c r="R24" s="38"/>
+      <c r="S24" s="38"/>
+      <c r="T24" s="38"/>
+      <c r="U24" s="38"/>
+      <c r="V24" s="38"/>
+      <c r="W24" s="38"/>
+      <c r="X24" s="38"/>
+      <c r="Y24" s="38"/>
+      <c r="Z24" s="38"/>
+      <c r="AA24" s="38"/>
+      <c r="AB24" s="38"/>
+      <c r="AC24" s="38"/>
+      <c r="AD24" s="38"/>
+      <c r="AE24" s="38"/>
+      <c r="AF24" s="38"/>
+      <c r="AG24" s="38"/>
+      <c r="AH24" s="38"/>
+      <c r="AI24" s="38"/>
+      <c r="AJ24" s="38"/>
+      <c r="AK24" s="38"/>
+      <c r="AL24" s="38"/>
+      <c r="AM24" s="38"/>
+      <c r="AN24" s="38"/>
+      <c r="AO24" s="38"/>
+      <c r="AP24" s="38"/>
+      <c r="AQ24" s="38"/>
+      <c r="AR24" s="38"/>
+      <c r="AS24" s="38"/>
+      <c r="AT24" s="38"/>
+      <c r="AU24" s="38"/>
+      <c r="AV24" s="38"/>
+      <c r="AW24" s="38"/>
+      <c r="AX24" s="38"/>
+      <c r="AY24" s="38"/>
+      <c r="AZ24" s="38"/>
+      <c r="BA24" s="38"/>
+      <c r="BB24" s="38"/>
+      <c r="BC24" s="38"/>
+      <c r="BD24" s="38"/>
+      <c r="BE24" s="38"/>
+      <c r="BF24" s="38"/>
+    </row>
+    <row r="25" spans="3:58" x14ac:dyDescent="0.25">
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
-      <c r="H25" s="59"/>
-      <c r="I25" s="59"/>
-      <c r="J25" s="59"/>
-      <c r="K25" s="59"/>
-      <c r="L25" s="59"/>
-      <c r="M25" s="59"/>
-      <c r="N25" s="59"/>
-      <c r="O25" s="59"/>
-      <c r="P25" s="59"/>
-      <c r="Q25" s="59"/>
-      <c r="R25" s="59"/>
-      <c r="S25" s="59"/>
-      <c r="T25" s="59"/>
-      <c r="U25" s="59"/>
-      <c r="V25" s="59"/>
-      <c r="W25" s="59"/>
-      <c r="X25" s="59"/>
-      <c r="Y25" s="59"/>
-      <c r="Z25" s="59"/>
-      <c r="AA25" s="59"/>
-      <c r="AB25" s="59"/>
-      <c r="AC25" s="59"/>
-      <c r="AD25" s="59"/>
-      <c r="AE25" s="59"/>
-      <c r="AF25" s="59"/>
-      <c r="AG25" s="59"/>
-      <c r="AH25" s="59"/>
-      <c r="AI25" s="59"/>
-      <c r="AJ25" s="59"/>
-      <c r="AK25" s="59"/>
-      <c r="AL25" s="59"/>
-      <c r="AM25" s="59"/>
-      <c r="AN25" s="59"/>
-      <c r="AO25" s="59"/>
-      <c r="AP25" s="59"/>
-      <c r="AQ25" s="59"/>
-      <c r="AR25" s="59"/>
-      <c r="AS25" s="59"/>
-      <c r="AT25" s="59"/>
-      <c r="AU25" s="59"/>
-      <c r="AV25" s="59"/>
-      <c r="AW25" s="59"/>
-      <c r="AX25" s="59"/>
-      <c r="AY25" s="59"/>
-      <c r="AZ25" s="59"/>
-      <c r="BA25" s="59"/>
-      <c r="BB25" s="59"/>
-      <c r="BC25" s="59"/>
-      <c r="BD25" s="59"/>
-      <c r="BE25" s="59"/>
-      <c r="BF25" s="59"/>
-    </row>
-    <row r="26" spans="3:58" x14ac:dyDescent="0.35">
+      <c r="H25" s="38"/>
+      <c r="I25" s="38"/>
+      <c r="J25" s="38"/>
+      <c r="K25" s="38"/>
+      <c r="L25" s="38"/>
+      <c r="M25" s="38"/>
+      <c r="N25" s="38"/>
+      <c r="O25" s="38"/>
+      <c r="P25" s="38"/>
+      <c r="Q25" s="38"/>
+      <c r="R25" s="38"/>
+      <c r="S25" s="38"/>
+      <c r="T25" s="38"/>
+      <c r="U25" s="38"/>
+      <c r="V25" s="38"/>
+      <c r="W25" s="38"/>
+      <c r="X25" s="38"/>
+      <c r="Y25" s="38"/>
+      <c r="Z25" s="38"/>
+      <c r="AA25" s="38"/>
+      <c r="AB25" s="38"/>
+      <c r="AC25" s="38"/>
+      <c r="AD25" s="38"/>
+      <c r="AE25" s="38"/>
+      <c r="AF25" s="38"/>
+      <c r="AG25" s="38"/>
+      <c r="AH25" s="38"/>
+      <c r="AI25" s="38"/>
+      <c r="AJ25" s="38"/>
+      <c r="AK25" s="38"/>
+      <c r="AL25" s="38"/>
+      <c r="AM25" s="38"/>
+      <c r="AN25" s="38"/>
+      <c r="AO25" s="38"/>
+      <c r="AP25" s="38"/>
+      <c r="AQ25" s="38"/>
+      <c r="AR25" s="38"/>
+      <c r="AS25" s="38"/>
+      <c r="AT25" s="38"/>
+      <c r="AU25" s="38"/>
+      <c r="AV25" s="38"/>
+      <c r="AW25" s="38"/>
+      <c r="AX25" s="38"/>
+      <c r="AY25" s="38"/>
+      <c r="AZ25" s="38"/>
+      <c r="BA25" s="38"/>
+      <c r="BB25" s="38"/>
+      <c r="BC25" s="38"/>
+      <c r="BD25" s="38"/>
+      <c r="BE25" s="38"/>
+      <c r="BF25" s="38"/>
+    </row>
+    <row r="26" spans="3:58" x14ac:dyDescent="0.25">
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
-      <c r="H26" s="59"/>
-      <c r="I26" s="59"/>
-      <c r="J26" s="59"/>
-      <c r="K26" s="59"/>
-      <c r="L26" s="59"/>
-      <c r="M26" s="59"/>
-      <c r="N26" s="59"/>
-      <c r="O26" s="59"/>
-      <c r="P26" s="59"/>
-      <c r="Q26" s="59"/>
-      <c r="R26" s="59"/>
-      <c r="S26" s="59"/>
-      <c r="T26" s="59"/>
-      <c r="U26" s="59"/>
-      <c r="V26" s="59"/>
-      <c r="W26" s="59"/>
-      <c r="X26" s="59"/>
-      <c r="Y26" s="59"/>
-      <c r="Z26" s="59"/>
-      <c r="AA26" s="59"/>
-      <c r="AB26" s="59"/>
-      <c r="AC26" s="59"/>
-      <c r="AD26" s="59"/>
-      <c r="AE26" s="59"/>
-      <c r="AF26" s="59"/>
-      <c r="AG26" s="59"/>
-      <c r="AH26" s="59"/>
-      <c r="AI26" s="59"/>
-      <c r="AJ26" s="59"/>
-      <c r="AK26" s="59"/>
-      <c r="AL26" s="59"/>
-      <c r="AM26" s="59"/>
-      <c r="AN26" s="59"/>
-      <c r="AO26" s="59"/>
-      <c r="AP26" s="59"/>
-      <c r="AQ26" s="59"/>
-      <c r="AR26" s="59"/>
-      <c r="AS26" s="59"/>
-      <c r="AT26" s="59"/>
-      <c r="AU26" s="59"/>
-      <c r="AV26" s="59"/>
-      <c r="AW26" s="59"/>
-      <c r="AX26" s="59"/>
-      <c r="AY26" s="59"/>
-      <c r="AZ26" s="59"/>
-      <c r="BA26" s="59"/>
-      <c r="BB26" s="59"/>
-      <c r="BC26" s="59"/>
-      <c r="BD26" s="59"/>
-      <c r="BE26" s="59"/>
-      <c r="BF26" s="59"/>
-    </row>
-    <row r="27" spans="3:58" ht="12.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H26" s="38"/>
+      <c r="I26" s="38"/>
+      <c r="J26" s="38"/>
+      <c r="K26" s="38"/>
+      <c r="L26" s="38"/>
+      <c r="M26" s="38"/>
+      <c r="N26" s="38"/>
+      <c r="O26" s="38"/>
+      <c r="P26" s="38"/>
+      <c r="Q26" s="38"/>
+      <c r="R26" s="38"/>
+      <c r="S26" s="38"/>
+      <c r="T26" s="38"/>
+      <c r="U26" s="38"/>
+      <c r="V26" s="38"/>
+      <c r="W26" s="38"/>
+      <c r="X26" s="38"/>
+      <c r="Y26" s="38"/>
+      <c r="Z26" s="38"/>
+      <c r="AA26" s="38"/>
+      <c r="AB26" s="38"/>
+      <c r="AC26" s="38"/>
+      <c r="AD26" s="38"/>
+      <c r="AE26" s="38"/>
+      <c r="AF26" s="38"/>
+      <c r="AG26" s="38"/>
+      <c r="AH26" s="38"/>
+      <c r="AI26" s="38"/>
+      <c r="AJ26" s="38"/>
+      <c r="AK26" s="38"/>
+      <c r="AL26" s="38"/>
+      <c r="AM26" s="38"/>
+      <c r="AN26" s="38"/>
+      <c r="AO26" s="38"/>
+      <c r="AP26" s="38"/>
+      <c r="AQ26" s="38"/>
+      <c r="AR26" s="38"/>
+      <c r="AS26" s="38"/>
+      <c r="AT26" s="38"/>
+      <c r="AU26" s="38"/>
+      <c r="AV26" s="38"/>
+      <c r="AW26" s="38"/>
+      <c r="AX26" s="38"/>
+      <c r="AY26" s="38"/>
+      <c r="AZ26" s="38"/>
+      <c r="BA26" s="38"/>
+      <c r="BB26" s="38"/>
+      <c r="BC26" s="38"/>
+      <c r="BD26" s="38"/>
+      <c r="BE26" s="38"/>
+      <c r="BF26" s="38"/>
+    </row>
+    <row r="27" spans="3:58" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
@@ -2470,7 +2540,7 @@
       <c r="BE27" s="1"/>
       <c r="BF27" s="1"/>
     </row>
-    <row r="28" spans="3:58" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="3:58" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
@@ -2482,61 +2552,61 @@
       <c r="I28" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="J28" s="60"/>
-      <c r="K28" s="60"/>
+      <c r="J28" s="39"/>
+      <c r="K28" s="39"/>
       <c r="L28" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="M28" s="51" t="s">
+      <c r="M28" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="N28" s="51"/>
-      <c r="O28" s="51"/>
-      <c r="P28" s="51"/>
-      <c r="Q28" s="51"/>
-      <c r="R28" s="51"/>
-      <c r="S28" s="51"/>
-      <c r="T28" s="51"/>
-      <c r="U28" s="51"/>
-      <c r="V28" s="51"/>
-      <c r="W28" s="51"/>
-      <c r="X28" s="51"/>
-      <c r="Y28" s="51"/>
-      <c r="Z28" s="51"/>
-      <c r="AA28" s="51"/>
-      <c r="AB28" s="51"/>
-      <c r="AC28" s="51"/>
-      <c r="AD28" s="51"/>
-      <c r="AE28" s="51"/>
-      <c r="AF28" s="51"/>
-      <c r="AG28" s="51"/>
-      <c r="AH28" s="51"/>
-      <c r="AI28" s="51"/>
-      <c r="AJ28" s="51"/>
-      <c r="AK28" s="51"/>
-      <c r="AL28" s="51"/>
-      <c r="AM28" s="51"/>
-      <c r="AN28" s="51"/>
-      <c r="AO28" s="51"/>
-      <c r="AP28" s="51"/>
-      <c r="AQ28" s="51"/>
-      <c r="AR28" s="51"/>
-      <c r="AS28" s="51"/>
-      <c r="AT28" s="51"/>
-      <c r="AU28" s="51"/>
-      <c r="AV28" s="51"/>
-      <c r="AW28" s="51"/>
-      <c r="AX28" s="51"/>
-      <c r="AY28" s="51"/>
-      <c r="AZ28" s="51"/>
-      <c r="BA28" s="51"/>
-      <c r="BB28" s="51"/>
-      <c r="BC28" s="51"/>
-      <c r="BD28" s="51"/>
-      <c r="BE28" s="51"/>
-      <c r="BF28" s="51"/>
-    </row>
-    <row r="29" spans="3:58" ht="77.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="N28" s="54"/>
+      <c r="O28" s="54"/>
+      <c r="P28" s="54"/>
+      <c r="Q28" s="54"/>
+      <c r="R28" s="54"/>
+      <c r="S28" s="54"/>
+      <c r="T28" s="54"/>
+      <c r="U28" s="54"/>
+      <c r="V28" s="54"/>
+      <c r="W28" s="54"/>
+      <c r="X28" s="54"/>
+      <c r="Y28" s="54"/>
+      <c r="Z28" s="54"/>
+      <c r="AA28" s="54"/>
+      <c r="AB28" s="54"/>
+      <c r="AC28" s="54"/>
+      <c r="AD28" s="54"/>
+      <c r="AE28" s="54"/>
+      <c r="AF28" s="54"/>
+      <c r="AG28" s="54"/>
+      <c r="AH28" s="54"/>
+      <c r="AI28" s="54"/>
+      <c r="AJ28" s="54"/>
+      <c r="AK28" s="54"/>
+      <c r="AL28" s="54"/>
+      <c r="AM28" s="54"/>
+      <c r="AN28" s="54"/>
+      <c r="AO28" s="54"/>
+      <c r="AP28" s="54"/>
+      <c r="AQ28" s="54"/>
+      <c r="AR28" s="54"/>
+      <c r="AS28" s="54"/>
+      <c r="AT28" s="54"/>
+      <c r="AU28" s="54"/>
+      <c r="AV28" s="54"/>
+      <c r="AW28" s="54"/>
+      <c r="AX28" s="54"/>
+      <c r="AY28" s="54"/>
+      <c r="AZ28" s="54"/>
+      <c r="BA28" s="54"/>
+      <c r="BB28" s="54"/>
+      <c r="BC28" s="54"/>
+      <c r="BD28" s="54"/>
+      <c r="BE28" s="54"/>
+      <c r="BF28" s="54"/>
+    </row>
+    <row r="29" spans="3:58" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -2547,54 +2617,54 @@
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
-      <c r="M29" s="51"/>
-      <c r="N29" s="51"/>
-      <c r="O29" s="51"/>
-      <c r="P29" s="51"/>
-      <c r="Q29" s="51"/>
-      <c r="R29" s="51"/>
-      <c r="S29" s="51"/>
-      <c r="T29" s="51"/>
-      <c r="U29" s="51"/>
-      <c r="V29" s="51"/>
-      <c r="W29" s="51"/>
-      <c r="X29" s="51"/>
-      <c r="Y29" s="51"/>
-      <c r="Z29" s="51"/>
-      <c r="AA29" s="51"/>
-      <c r="AB29" s="51"/>
-      <c r="AC29" s="51"/>
-      <c r="AD29" s="51"/>
-      <c r="AE29" s="51"/>
-      <c r="AF29" s="51"/>
-      <c r="AG29" s="51"/>
-      <c r="AH29" s="51"/>
-      <c r="AI29" s="51"/>
-      <c r="AJ29" s="51"/>
-      <c r="AK29" s="51"/>
-      <c r="AL29" s="51"/>
-      <c r="AM29" s="51"/>
-      <c r="AN29" s="51"/>
-      <c r="AO29" s="51"/>
-      <c r="AP29" s="51"/>
-      <c r="AQ29" s="51"/>
-      <c r="AR29" s="51"/>
-      <c r="AS29" s="51"/>
-      <c r="AT29" s="51"/>
-      <c r="AU29" s="51"/>
-      <c r="AV29" s="51"/>
-      <c r="AW29" s="51"/>
-      <c r="AX29" s="51"/>
-      <c r="AY29" s="51"/>
-      <c r="AZ29" s="51"/>
-      <c r="BA29" s="51"/>
-      <c r="BB29" s="51"/>
-      <c r="BC29" s="51"/>
-      <c r="BD29" s="51"/>
-      <c r="BE29" s="51"/>
-      <c r="BF29" s="51"/>
-    </row>
-    <row r="30" spans="3:58" ht="12.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="M29" s="54"/>
+      <c r="N29" s="54"/>
+      <c r="O29" s="54"/>
+      <c r="P29" s="54"/>
+      <c r="Q29" s="54"/>
+      <c r="R29" s="54"/>
+      <c r="S29" s="54"/>
+      <c r="T29" s="54"/>
+      <c r="U29" s="54"/>
+      <c r="V29" s="54"/>
+      <c r="W29" s="54"/>
+      <c r="X29" s="54"/>
+      <c r="Y29" s="54"/>
+      <c r="Z29" s="54"/>
+      <c r="AA29" s="54"/>
+      <c r="AB29" s="54"/>
+      <c r="AC29" s="54"/>
+      <c r="AD29" s="54"/>
+      <c r="AE29" s="54"/>
+      <c r="AF29" s="54"/>
+      <c r="AG29" s="54"/>
+      <c r="AH29" s="54"/>
+      <c r="AI29" s="54"/>
+      <c r="AJ29" s="54"/>
+      <c r="AK29" s="54"/>
+      <c r="AL29" s="54"/>
+      <c r="AM29" s="54"/>
+      <c r="AN29" s="54"/>
+      <c r="AO29" s="54"/>
+      <c r="AP29" s="54"/>
+      <c r="AQ29" s="54"/>
+      <c r="AR29" s="54"/>
+      <c r="AS29" s="54"/>
+      <c r="AT29" s="54"/>
+      <c r="AU29" s="54"/>
+      <c r="AV29" s="54"/>
+      <c r="AW29" s="54"/>
+      <c r="AX29" s="54"/>
+      <c r="AY29" s="54"/>
+      <c r="AZ29" s="54"/>
+      <c r="BA29" s="54"/>
+      <c r="BB29" s="54"/>
+      <c r="BC29" s="54"/>
+      <c r="BD29" s="54"/>
+      <c r="BE29" s="54"/>
+      <c r="BF29" s="54"/>
+    </row>
+    <row r="30" spans="3:58" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
@@ -2652,7 +2722,7 @@
       <c r="BE30" s="1"/>
       <c r="BF30" s="1"/>
     </row>
-    <row r="31" spans="3:58" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="3:58" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
@@ -2664,61 +2734,61 @@
       <c r="I31" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="J31" s="60"/>
-      <c r="K31" s="60"/>
+      <c r="J31" s="39"/>
+      <c r="K31" s="39"/>
       <c r="L31" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="M31" s="51" t="s">
+      <c r="M31" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="N31" s="51"/>
-      <c r="O31" s="51"/>
-      <c r="P31" s="51"/>
-      <c r="Q31" s="51"/>
-      <c r="R31" s="51"/>
-      <c r="S31" s="51"/>
-      <c r="T31" s="51"/>
-      <c r="U31" s="51"/>
-      <c r="V31" s="51"/>
-      <c r="W31" s="51"/>
-      <c r="X31" s="51"/>
-      <c r="Y31" s="51"/>
-      <c r="Z31" s="51"/>
-      <c r="AA31" s="51"/>
-      <c r="AB31" s="51"/>
-      <c r="AC31" s="51"/>
-      <c r="AD31" s="51"/>
-      <c r="AE31" s="51"/>
-      <c r="AF31" s="51"/>
-      <c r="AG31" s="51"/>
-      <c r="AH31" s="51"/>
-      <c r="AI31" s="51"/>
-      <c r="AJ31" s="51"/>
-      <c r="AK31" s="51"/>
-      <c r="AL31" s="51"/>
-      <c r="AM31" s="51"/>
-      <c r="AN31" s="51"/>
-      <c r="AO31" s="51"/>
-      <c r="AP31" s="51"/>
-      <c r="AQ31" s="51"/>
-      <c r="AR31" s="51"/>
-      <c r="AS31" s="51"/>
-      <c r="AT31" s="51"/>
-      <c r="AU31" s="51"/>
-      <c r="AV31" s="51"/>
-      <c r="AW31" s="51"/>
-      <c r="AX31" s="51"/>
-      <c r="AY31" s="51"/>
-      <c r="AZ31" s="51"/>
-      <c r="BA31" s="51"/>
-      <c r="BB31" s="51"/>
-      <c r="BC31" s="51"/>
-      <c r="BD31" s="51"/>
-      <c r="BE31" s="51"/>
-      <c r="BF31" s="51"/>
-    </row>
-    <row r="32" spans="3:58" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="N31" s="54"/>
+      <c r="O31" s="54"/>
+      <c r="P31" s="54"/>
+      <c r="Q31" s="54"/>
+      <c r="R31" s="54"/>
+      <c r="S31" s="54"/>
+      <c r="T31" s="54"/>
+      <c r="U31" s="54"/>
+      <c r="V31" s="54"/>
+      <c r="W31" s="54"/>
+      <c r="X31" s="54"/>
+      <c r="Y31" s="54"/>
+      <c r="Z31" s="54"/>
+      <c r="AA31" s="54"/>
+      <c r="AB31" s="54"/>
+      <c r="AC31" s="54"/>
+      <c r="AD31" s="54"/>
+      <c r="AE31" s="54"/>
+      <c r="AF31" s="54"/>
+      <c r="AG31" s="54"/>
+      <c r="AH31" s="54"/>
+      <c r="AI31" s="54"/>
+      <c r="AJ31" s="54"/>
+      <c r="AK31" s="54"/>
+      <c r="AL31" s="54"/>
+      <c r="AM31" s="54"/>
+      <c r="AN31" s="54"/>
+      <c r="AO31" s="54"/>
+      <c r="AP31" s="54"/>
+      <c r="AQ31" s="54"/>
+      <c r="AR31" s="54"/>
+      <c r="AS31" s="54"/>
+      <c r="AT31" s="54"/>
+      <c r="AU31" s="54"/>
+      <c r="AV31" s="54"/>
+      <c r="AW31" s="54"/>
+      <c r="AX31" s="54"/>
+      <c r="AY31" s="54"/>
+      <c r="AZ31" s="54"/>
+      <c r="BA31" s="54"/>
+      <c r="BB31" s="54"/>
+      <c r="BC31" s="54"/>
+      <c r="BD31" s="54"/>
+      <c r="BE31" s="54"/>
+      <c r="BF31" s="54"/>
+    </row>
+    <row r="32" spans="3:58" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
@@ -2729,54 +2799,54 @@
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
-      <c r="M32" s="51"/>
-      <c r="N32" s="51"/>
-      <c r="O32" s="51"/>
-      <c r="P32" s="51"/>
-      <c r="Q32" s="51"/>
-      <c r="R32" s="51"/>
-      <c r="S32" s="51"/>
-      <c r="T32" s="51"/>
-      <c r="U32" s="51"/>
-      <c r="V32" s="51"/>
-      <c r="W32" s="51"/>
-      <c r="X32" s="51"/>
-      <c r="Y32" s="51"/>
-      <c r="Z32" s="51"/>
-      <c r="AA32" s="51"/>
-      <c r="AB32" s="51"/>
-      <c r="AC32" s="51"/>
-      <c r="AD32" s="51"/>
-      <c r="AE32" s="51"/>
-      <c r="AF32" s="51"/>
-      <c r="AG32" s="51"/>
-      <c r="AH32" s="51"/>
-      <c r="AI32" s="51"/>
-      <c r="AJ32" s="51"/>
-      <c r="AK32" s="51"/>
-      <c r="AL32" s="51"/>
-      <c r="AM32" s="51"/>
-      <c r="AN32" s="51"/>
-      <c r="AO32" s="51"/>
-      <c r="AP32" s="51"/>
-      <c r="AQ32" s="51"/>
-      <c r="AR32" s="51"/>
-      <c r="AS32" s="51"/>
-      <c r="AT32" s="51"/>
-      <c r="AU32" s="51"/>
-      <c r="AV32" s="51"/>
-      <c r="AW32" s="51"/>
-      <c r="AX32" s="51"/>
-      <c r="AY32" s="51"/>
-      <c r="AZ32" s="51"/>
-      <c r="BA32" s="51"/>
-      <c r="BB32" s="51"/>
-      <c r="BC32" s="51"/>
-      <c r="BD32" s="51"/>
-      <c r="BE32" s="51"/>
-      <c r="BF32" s="51"/>
-    </row>
-    <row r="33" spans="3:58" x14ac:dyDescent="0.35">
+      <c r="M32" s="54"/>
+      <c r="N32" s="54"/>
+      <c r="O32" s="54"/>
+      <c r="P32" s="54"/>
+      <c r="Q32" s="54"/>
+      <c r="R32" s="54"/>
+      <c r="S32" s="54"/>
+      <c r="T32" s="54"/>
+      <c r="U32" s="54"/>
+      <c r="V32" s="54"/>
+      <c r="W32" s="54"/>
+      <c r="X32" s="54"/>
+      <c r="Y32" s="54"/>
+      <c r="Z32" s="54"/>
+      <c r="AA32" s="54"/>
+      <c r="AB32" s="54"/>
+      <c r="AC32" s="54"/>
+      <c r="AD32" s="54"/>
+      <c r="AE32" s="54"/>
+      <c r="AF32" s="54"/>
+      <c r="AG32" s="54"/>
+      <c r="AH32" s="54"/>
+      <c r="AI32" s="54"/>
+      <c r="AJ32" s="54"/>
+      <c r="AK32" s="54"/>
+      <c r="AL32" s="54"/>
+      <c r="AM32" s="54"/>
+      <c r="AN32" s="54"/>
+      <c r="AO32" s="54"/>
+      <c r="AP32" s="54"/>
+      <c r="AQ32" s="54"/>
+      <c r="AR32" s="54"/>
+      <c r="AS32" s="54"/>
+      <c r="AT32" s="54"/>
+      <c r="AU32" s="54"/>
+      <c r="AV32" s="54"/>
+      <c r="AW32" s="54"/>
+      <c r="AX32" s="54"/>
+      <c r="AY32" s="54"/>
+      <c r="AZ32" s="54"/>
+      <c r="BA32" s="54"/>
+      <c r="BB32" s="54"/>
+      <c r="BC32" s="54"/>
+      <c r="BD32" s="54"/>
+      <c r="BE32" s="54"/>
+      <c r="BF32" s="54"/>
+    </row>
+    <row r="33" spans="3:58" x14ac:dyDescent="0.25">
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
@@ -2787,56 +2857,56 @@
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
-      <c r="M33" s="49" t="s">
+      <c r="M33" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="N33" s="49"/>
-      <c r="O33" s="49"/>
-      <c r="P33" s="49"/>
-      <c r="Q33" s="49"/>
-      <c r="R33" s="49"/>
-      <c r="S33" s="49"/>
-      <c r="T33" s="49"/>
-      <c r="U33" s="49"/>
-      <c r="V33" s="49"/>
-      <c r="W33" s="63"/>
-      <c r="X33" s="63"/>
-      <c r="Y33" s="63"/>
-      <c r="Z33" s="63"/>
-      <c r="AA33" s="63"/>
-      <c r="AB33" s="63"/>
-      <c r="AC33" s="63"/>
-      <c r="AD33" s="63"/>
-      <c r="AE33" s="63"/>
-      <c r="AF33" s="63"/>
-      <c r="AG33" s="63"/>
-      <c r="AH33" s="63"/>
-      <c r="AI33" s="63"/>
-      <c r="AJ33" s="63"/>
-      <c r="AK33" s="63"/>
-      <c r="AL33" s="63"/>
-      <c r="AM33" s="63"/>
-      <c r="AN33" s="63"/>
-      <c r="AO33" s="63"/>
-      <c r="AP33" s="63"/>
-      <c r="AQ33" s="63"/>
-      <c r="AR33" s="63"/>
-      <c r="AS33" s="63"/>
-      <c r="AT33" s="63"/>
-      <c r="AU33" s="63"/>
-      <c r="AV33" s="63"/>
-      <c r="AW33" s="63"/>
-      <c r="AX33" s="63"/>
-      <c r="AY33" s="63"/>
-      <c r="AZ33" s="63"/>
-      <c r="BA33" s="63"/>
-      <c r="BB33" s="63"/>
-      <c r="BC33" s="63"/>
-      <c r="BD33" s="63"/>
-      <c r="BE33" s="63"/>
-      <c r="BF33" s="63"/>
-    </row>
-    <row r="34" spans="3:58" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="N33" s="52"/>
+      <c r="O33" s="52"/>
+      <c r="P33" s="52"/>
+      <c r="Q33" s="52"/>
+      <c r="R33" s="52"/>
+      <c r="S33" s="52"/>
+      <c r="T33" s="52"/>
+      <c r="U33" s="52"/>
+      <c r="V33" s="52"/>
+      <c r="W33" s="42"/>
+      <c r="X33" s="42"/>
+      <c r="Y33" s="42"/>
+      <c r="Z33" s="42"/>
+      <c r="AA33" s="42"/>
+      <c r="AB33" s="42"/>
+      <c r="AC33" s="42"/>
+      <c r="AD33" s="42"/>
+      <c r="AE33" s="42"/>
+      <c r="AF33" s="42"/>
+      <c r="AG33" s="42"/>
+      <c r="AH33" s="42"/>
+      <c r="AI33" s="42"/>
+      <c r="AJ33" s="42"/>
+      <c r="AK33" s="42"/>
+      <c r="AL33" s="42"/>
+      <c r="AM33" s="42"/>
+      <c r="AN33" s="42"/>
+      <c r="AO33" s="42"/>
+      <c r="AP33" s="42"/>
+      <c r="AQ33" s="42"/>
+      <c r="AR33" s="42"/>
+      <c r="AS33" s="42"/>
+      <c r="AT33" s="42"/>
+      <c r="AU33" s="42"/>
+      <c r="AV33" s="42"/>
+      <c r="AW33" s="42"/>
+      <c r="AX33" s="42"/>
+      <c r="AY33" s="42"/>
+      <c r="AZ33" s="42"/>
+      <c r="BA33" s="42"/>
+      <c r="BB33" s="42"/>
+      <c r="BC33" s="42"/>
+      <c r="BD33" s="42"/>
+      <c r="BE33" s="42"/>
+      <c r="BF33" s="42"/>
+    </row>
+    <row r="34" spans="3:58" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
@@ -2894,7 +2964,7 @@
       <c r="BE34" s="15"/>
       <c r="BF34" s="15"/>
     </row>
-    <row r="35" spans="3:58" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="3:58" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
@@ -2905,68 +2975,68 @@
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
-      <c r="M35" s="52" t="s">
+      <c r="M35" s="55" t="s">
         <v>25</v>
       </c>
-      <c r="N35" s="52"/>
-      <c r="O35" s="52"/>
-      <c r="P35" s="52"/>
-      <c r="Q35" s="52"/>
-      <c r="R35" s="52"/>
-      <c r="S35" s="52"/>
-      <c r="T35" s="52"/>
-      <c r="U35" s="52"/>
-      <c r="V35" s="52"/>
-      <c r="W35" s="52"/>
-      <c r="X35" s="52"/>
-      <c r="Y35" s="52"/>
-      <c r="Z35" s="52"/>
-      <c r="AA35" s="52"/>
-      <c r="AB35" s="52"/>
-      <c r="AC35" s="52"/>
-      <c r="AD35" s="52"/>
-      <c r="AE35" s="52"/>
-      <c r="AF35" s="52"/>
-      <c r="AG35" s="52"/>
-      <c r="AH35" s="52"/>
-      <c r="AI35" s="52"/>
-      <c r="AJ35" s="52"/>
-      <c r="AK35" s="52"/>
-      <c r="AL35" s="52"/>
-      <c r="AM35" s="52"/>
-      <c r="AN35" s="52"/>
+      <c r="N35" s="55"/>
+      <c r="O35" s="55"/>
+      <c r="P35" s="55"/>
+      <c r="Q35" s="55"/>
+      <c r="R35" s="55"/>
+      <c r="S35" s="55"/>
+      <c r="T35" s="55"/>
+      <c r="U35" s="55"/>
+      <c r="V35" s="55"/>
+      <c r="W35" s="55"/>
+      <c r="X35" s="55"/>
+      <c r="Y35" s="55"/>
+      <c r="Z35" s="55"/>
+      <c r="AA35" s="55"/>
+      <c r="AB35" s="55"/>
+      <c r="AC35" s="55"/>
+      <c r="AD35" s="55"/>
+      <c r="AE35" s="55"/>
+      <c r="AF35" s="55"/>
+      <c r="AG35" s="55"/>
+      <c r="AH35" s="55"/>
+      <c r="AI35" s="55"/>
+      <c r="AJ35" s="55"/>
+      <c r="AK35" s="55"/>
+      <c r="AL35" s="55"/>
+      <c r="AM35" s="55"/>
+      <c r="AN35" s="55"/>
       <c r="AO35" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="AP35" s="61"/>
-      <c r="AQ35" s="61"/>
+      <c r="AP35" s="40"/>
+      <c r="AQ35" s="40"/>
       <c r="AR35" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="AS35" s="64" t="s">
+      <c r="AS35" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="AT35" s="64"/>
-      <c r="AU35" s="64"/>
+      <c r="AT35" s="43"/>
+      <c r="AU35" s="43"/>
       <c r="AV35" s="1"/>
       <c r="AW35" s="17"/>
       <c r="AX35" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="AY35" s="61"/>
-      <c r="AZ35" s="61"/>
+      <c r="AY35" s="40"/>
+      <c r="AZ35" s="40"/>
       <c r="BA35" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="BB35" s="50" t="s">
+      <c r="BB35" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="BC35" s="50"/>
-      <c r="BD35" s="50"/>
+      <c r="BC35" s="53"/>
+      <c r="BD35" s="53"/>
       <c r="BE35" s="19"/>
       <c r="BF35" s="17"/>
     </row>
-    <row r="36" spans="3:58" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="3:58" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
@@ -3024,7 +3094,7 @@
       <c r="BE36" s="1"/>
       <c r="BF36" s="1"/>
     </row>
-    <row r="37" spans="3:58" x14ac:dyDescent="0.35">
+    <row r="37" spans="3:58" x14ac:dyDescent="0.25">
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
@@ -3061,36 +3131,42 @@
       <c r="AH37" s="1"/>
       <c r="AI37" s="1"/>
       <c r="AJ37" s="1"/>
-      <c r="AK37" s="62"/>
-      <c r="AL37" s="62"/>
+      <c r="AK37" s="41" t="s">
+        <v>50</v>
+      </c>
+      <c r="AL37" s="41"/>
       <c r="AM37" s="1" t="s">
         <v>17</v>
       </c>
       <c r="AN37" s="1"/>
-      <c r="AO37" s="61"/>
-      <c r="AP37" s="61"/>
-      <c r="AQ37" s="61"/>
-      <c r="AR37" s="61"/>
-      <c r="AS37" s="61"/>
-      <c r="AT37" s="61"/>
-      <c r="AU37" s="61"/>
-      <c r="AV37" s="61"/>
+      <c r="AO37" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="AP37" s="40"/>
+      <c r="AQ37" s="40"/>
+      <c r="AR37" s="40"/>
+      <c r="AS37" s="40"/>
+      <c r="AT37" s="40"/>
+      <c r="AU37" s="40"/>
+      <c r="AV37" s="40"/>
       <c r="AW37" s="20" t="s">
         <v>17</v>
       </c>
       <c r="AX37" s="1"/>
-      <c r="AY37" s="61"/>
-      <c r="AZ37" s="61"/>
-      <c r="BA37" s="61"/>
-      <c r="BB37" s="61"/>
-      <c r="BC37" s="61"/>
-      <c r="BD37" s="61"/>
-      <c r="BE37" s="61"/>
+      <c r="AY37" s="40">
+        <v>2018</v>
+      </c>
+      <c r="AZ37" s="40"/>
+      <c r="BA37" s="40"/>
+      <c r="BB37" s="40"/>
+      <c r="BC37" s="40"/>
+      <c r="BD37" s="40"/>
+      <c r="BE37" s="40"/>
       <c r="BF37" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="3:58" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="3:58" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AK38" s="1"/>
       <c r="AL38" s="1"/>
       <c r="AO38" s="1"/>
@@ -3109,68 +3185,68 @@
       <c r="BD38" s="1"/>
       <c r="BE38" s="1"/>
     </row>
-    <row r="39" spans="3:58" x14ac:dyDescent="0.35">
+    <row r="39" spans="3:58" x14ac:dyDescent="0.25">
       <c r="C39" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="P39" s="43" t="s">
+      <c r="P39" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="Q39" s="43"/>
-      <c r="R39" s="43"/>
-      <c r="S39" s="43"/>
-      <c r="T39" s="43"/>
-      <c r="U39" s="43"/>
-      <c r="V39" s="43"/>
-      <c r="W39" s="43"/>
-      <c r="X39" s="43"/>
-      <c r="Y39" s="43"/>
-      <c r="Z39" s="43"/>
-      <c r="AA39" s="43"/>
-      <c r="AB39" s="43"/>
-      <c r="AC39" s="43"/>
-      <c r="AD39" s="43"/>
-      <c r="AE39" s="43"/>
-      <c r="AF39" s="43"/>
-      <c r="AG39" s="43"/>
-      <c r="AH39" s="43"/>
-      <c r="AI39" s="43"/>
-      <c r="AJ39" s="43"/>
-      <c r="AK39" s="43"/>
-      <c r="AL39" s="43"/>
-    </row>
-    <row r="40" spans="3:58" ht="23.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="41" spans="3:58" x14ac:dyDescent="0.35">
+      <c r="Q39" s="59"/>
+      <c r="R39" s="59"/>
+      <c r="S39" s="59"/>
+      <c r="T39" s="59"/>
+      <c r="U39" s="59"/>
+      <c r="V39" s="59"/>
+      <c r="W39" s="59"/>
+      <c r="X39" s="59"/>
+      <c r="Y39" s="59"/>
+      <c r="Z39" s="59"/>
+      <c r="AA39" s="59"/>
+      <c r="AB39" s="59"/>
+      <c r="AC39" s="59"/>
+      <c r="AD39" s="59"/>
+      <c r="AE39" s="59"/>
+      <c r="AF39" s="59"/>
+      <c r="AG39" s="59"/>
+      <c r="AH39" s="59"/>
+      <c r="AI39" s="59"/>
+      <c r="AJ39" s="59"/>
+      <c r="AK39" s="59"/>
+      <c r="AL39" s="59"/>
+    </row>
+    <row r="40" spans="3:58" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="3:58" x14ac:dyDescent="0.25">
       <c r="C41" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="P41" s="65" t="s">
+      <c r="P41" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="Q41" s="65"/>
-      <c r="R41" s="65"/>
-      <c r="S41" s="65"/>
-      <c r="T41" s="65"/>
-      <c r="U41" s="65"/>
-      <c r="V41" s="65"/>
-      <c r="W41" s="65"/>
-      <c r="X41" s="65"/>
-      <c r="Y41" s="65"/>
-      <c r="Z41" s="65"/>
-      <c r="AA41" s="65"/>
-      <c r="AB41" s="65"/>
-      <c r="AC41" s="65"/>
-      <c r="AD41" s="65"/>
-      <c r="AE41" s="65"/>
-      <c r="AF41" s="65"/>
-      <c r="AG41" s="65"/>
-      <c r="AH41" s="65"/>
-      <c r="AI41" s="65"/>
-      <c r="AJ41" s="65"/>
-      <c r="AK41" s="65"/>
-      <c r="AL41" s="65"/>
-    </row>
-    <row r="42" spans="3:58" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q41" s="44"/>
+      <c r="R41" s="44"/>
+      <c r="S41" s="44"/>
+      <c r="T41" s="44"/>
+      <c r="U41" s="44"/>
+      <c r="V41" s="44"/>
+      <c r="W41" s="44"/>
+      <c r="X41" s="44"/>
+      <c r="Y41" s="44"/>
+      <c r="Z41" s="44"/>
+      <c r="AA41" s="44"/>
+      <c r="AB41" s="44"/>
+      <c r="AC41" s="44"/>
+      <c r="AD41" s="44"/>
+      <c r="AE41" s="44"/>
+      <c r="AF41" s="44"/>
+      <c r="AG41" s="44"/>
+      <c r="AH41" s="44"/>
+      <c r="AI41" s="44"/>
+      <c r="AJ41" s="44"/>
+      <c r="AK41" s="44"/>
+      <c r="AL41" s="44"/>
+    </row>
+    <row r="42" spans="3:58" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C42" s="9"/>
       <c r="D42" s="9"/>
       <c r="E42" s="9"/>
@@ -3228,67 +3304,67 @@
       <c r="BE42" s="9"/>
       <c r="BF42" s="9"/>
     </row>
-    <row r="43" spans="3:58" ht="84.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C43" s="57" t="s">
+    <row r="43" spans="3:58" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C43" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="D43" s="57"/>
-      <c r="E43" s="57"/>
-      <c r="F43" s="57"/>
-      <c r="G43" s="57"/>
-      <c r="H43" s="57"/>
-      <c r="I43" s="57"/>
-      <c r="J43" s="57"/>
-      <c r="K43" s="57"/>
-      <c r="L43" s="57"/>
-      <c r="M43" s="57"/>
-      <c r="N43" s="57"/>
-      <c r="O43" s="57"/>
-      <c r="P43" s="57"/>
-      <c r="Q43" s="57"/>
-      <c r="R43" s="57"/>
-      <c r="S43" s="57"/>
-      <c r="T43" s="57"/>
-      <c r="U43" s="57"/>
-      <c r="V43" s="57"/>
-      <c r="W43" s="57"/>
-      <c r="X43" s="57"/>
-      <c r="Y43" s="57"/>
-      <c r="Z43" s="57"/>
-      <c r="AA43" s="57"/>
-      <c r="AB43" s="57"/>
-      <c r="AC43" s="57"/>
-      <c r="AD43" s="57"/>
-      <c r="AE43" s="57"/>
-      <c r="AF43" s="57"/>
-      <c r="AG43" s="57"/>
-      <c r="AH43" s="57"/>
-      <c r="AI43" s="57"/>
-      <c r="AJ43" s="57"/>
-      <c r="AK43" s="57"/>
-      <c r="AL43" s="57"/>
-      <c r="AM43" s="57"/>
-      <c r="AN43" s="57"/>
-      <c r="AO43" s="57"/>
-      <c r="AP43" s="57"/>
-      <c r="AQ43" s="57"/>
-      <c r="AR43" s="57"/>
-      <c r="AS43" s="57"/>
-      <c r="AT43" s="57"/>
-      <c r="AU43" s="57"/>
-      <c r="AV43" s="57"/>
-      <c r="AW43" s="57"/>
-      <c r="AX43" s="57"/>
-      <c r="AY43" s="57"/>
-      <c r="AZ43" s="57"/>
-      <c r="BA43" s="57"/>
-      <c r="BB43" s="57"/>
-      <c r="BC43" s="57"/>
-      <c r="BD43" s="57"/>
-      <c r="BE43" s="57"/>
-      <c r="BF43" s="57"/>
-    </row>
-    <row r="44" spans="3:58" x14ac:dyDescent="0.35">
+      <c r="D43" s="36"/>
+      <c r="E43" s="36"/>
+      <c r="F43" s="36"/>
+      <c r="G43" s="36"/>
+      <c r="H43" s="36"/>
+      <c r="I43" s="36"/>
+      <c r="J43" s="36"/>
+      <c r="K43" s="36"/>
+      <c r="L43" s="36"/>
+      <c r="M43" s="36"/>
+      <c r="N43" s="36"/>
+      <c r="O43" s="36"/>
+      <c r="P43" s="36"/>
+      <c r="Q43" s="36"/>
+      <c r="R43" s="36"/>
+      <c r="S43" s="36"/>
+      <c r="T43" s="36"/>
+      <c r="U43" s="36"/>
+      <c r="V43" s="36"/>
+      <c r="W43" s="36"/>
+      <c r="X43" s="36"/>
+      <c r="Y43" s="36"/>
+      <c r="Z43" s="36"/>
+      <c r="AA43" s="36"/>
+      <c r="AB43" s="36"/>
+      <c r="AC43" s="36"/>
+      <c r="AD43" s="36"/>
+      <c r="AE43" s="36"/>
+      <c r="AF43" s="36"/>
+      <c r="AG43" s="36"/>
+      <c r="AH43" s="36"/>
+      <c r="AI43" s="36"/>
+      <c r="AJ43" s="36"/>
+      <c r="AK43" s="36"/>
+      <c r="AL43" s="36"/>
+      <c r="AM43" s="36"/>
+      <c r="AN43" s="36"/>
+      <c r="AO43" s="36"/>
+      <c r="AP43" s="36"/>
+      <c r="AQ43" s="36"/>
+      <c r="AR43" s="36"/>
+      <c r="AS43" s="36"/>
+      <c r="AT43" s="36"/>
+      <c r="AU43" s="36"/>
+      <c r="AV43" s="36"/>
+      <c r="AW43" s="36"/>
+      <c r="AX43" s="36"/>
+      <c r="AY43" s="36"/>
+      <c r="AZ43" s="36"/>
+      <c r="BA43" s="36"/>
+      <c r="BB43" s="36"/>
+      <c r="BC43" s="36"/>
+      <c r="BD43" s="36"/>
+      <c r="BE43" s="36"/>
+      <c r="BF43" s="36"/>
+    </row>
+    <row r="44" spans="3:58" x14ac:dyDescent="0.25">
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
@@ -3346,7 +3422,7 @@
       <c r="BE44" s="3"/>
       <c r="BF44" s="3"/>
     </row>
-    <row r="45" spans="3:58" x14ac:dyDescent="0.35">
+    <row r="45" spans="3:58" x14ac:dyDescent="0.25">
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
@@ -3404,7 +3480,7 @@
       <c r="BE45" s="3"/>
       <c r="BF45" s="3"/>
     </row>
-    <row r="46" spans="3:58" x14ac:dyDescent="0.35">
+    <row r="46" spans="3:58" x14ac:dyDescent="0.25">
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
@@ -3462,7 +3538,7 @@
       <c r="BE46" s="2"/>
       <c r="BF46" s="2"/>
     </row>
-    <row r="47" spans="3:58" x14ac:dyDescent="0.35">
+    <row r="47" spans="3:58" x14ac:dyDescent="0.25">
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
@@ -3523,28 +3599,19 @@
   </sheetData>
   <sheetProtection password="CEEB" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="51">
-    <mergeCell ref="C43:BF43"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="H19:BF21"/>
-    <mergeCell ref="H23:BF26"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="AY37:BE37"/>
-    <mergeCell ref="AK37:AL37"/>
-    <mergeCell ref="AY35:AZ35"/>
-    <mergeCell ref="W33:BF33"/>
-    <mergeCell ref="AS35:AU35"/>
-    <mergeCell ref="AP35:AQ35"/>
-    <mergeCell ref="P41:AL41"/>
-    <mergeCell ref="AO37:AV37"/>
-    <mergeCell ref="C5:H5"/>
-    <mergeCell ref="I5:U5"/>
-    <mergeCell ref="AJ9:BF9"/>
-    <mergeCell ref="AF9:AH9"/>
-    <mergeCell ref="H9:Y9"/>
-    <mergeCell ref="AC5:AQ5"/>
-    <mergeCell ref="AA9:AE9"/>
+    <mergeCell ref="BI13:BJ13"/>
+    <mergeCell ref="S15:AB15"/>
+    <mergeCell ref="C14:BF14"/>
+    <mergeCell ref="AC15:BF15"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="O17:R17"/>
+    <mergeCell ref="AU3:BE3"/>
+    <mergeCell ref="AR5:BF5"/>
+    <mergeCell ref="P39:AL39"/>
+    <mergeCell ref="AV17:AW17"/>
+    <mergeCell ref="AY17:AZ17"/>
+    <mergeCell ref="BB17:BE17"/>
     <mergeCell ref="C11:L11"/>
     <mergeCell ref="M11:BF11"/>
     <mergeCell ref="C1:BF1"/>
@@ -3561,19 +3628,28 @@
     <mergeCell ref="C13:BF13"/>
     <mergeCell ref="E3:AJ3"/>
     <mergeCell ref="AL3:AT3"/>
-    <mergeCell ref="AU3:BE3"/>
-    <mergeCell ref="AR5:BF5"/>
-    <mergeCell ref="P39:AL39"/>
-    <mergeCell ref="AV17:AW17"/>
-    <mergeCell ref="AY17:AZ17"/>
-    <mergeCell ref="BB17:BE17"/>
-    <mergeCell ref="BI13:BJ13"/>
-    <mergeCell ref="S15:AB15"/>
-    <mergeCell ref="C14:BF14"/>
-    <mergeCell ref="AC15:BF15"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="O17:R17"/>
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="I5:U5"/>
+    <mergeCell ref="AJ9:BF9"/>
+    <mergeCell ref="AF9:AH9"/>
+    <mergeCell ref="H9:Y9"/>
+    <mergeCell ref="AC5:AQ5"/>
+    <mergeCell ref="AA9:AE9"/>
+    <mergeCell ref="C43:BF43"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="H19:BF21"/>
+    <mergeCell ref="H23:BF26"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="AY37:BE37"/>
+    <mergeCell ref="AK37:AL37"/>
+    <mergeCell ref="AY35:AZ35"/>
+    <mergeCell ref="W33:BF33"/>
+    <mergeCell ref="AS35:AU35"/>
+    <mergeCell ref="AP35:AQ35"/>
+    <mergeCell ref="P41:AL41"/>
+    <mergeCell ref="AO37:AV37"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:AJ3">
     <cfRule type="notContainsBlanks" dxfId="11" priority="16">

</xml_diff>